<commit_message>
Renamed the settings column in DSPP to Setting, since Default crashed with the SQLite parser
</commit_message>
<xml_diff>
--- a/inst/default_parameters.xlsx
+++ b/inst/default_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frkkan96/Documents/src/reindeer/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74FC03D-14EE-0647-824C-BF22B069C937}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FDE29B-BD82-9347-910F-8755C7568729}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25620" yWindow="500" windowWidth="25580" windowHeight="28300" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
   </bookViews>
@@ -63,9 +63,6 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>Default</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
@@ -115,6 +112,9 @@
   </si>
   <si>
     <t>maxhzformant</t>
+  </si>
+  <si>
+    <t>Setting</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <dimension ref="A1:E72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="209" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,16 +510,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -527,50 +527,50 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -578,13 +578,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1">
         <v>400</v>
@@ -592,16 +592,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1">
         <v>640</v>
@@ -609,16 +609,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1">
         <v>600</v>
@@ -629,13 +629,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1">
         <v>50</v>
@@ -643,16 +643,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="1">
         <v>80</v>
@@ -660,16 +660,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E10" s="1">
         <v>50</v>
@@ -680,13 +680,13 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="1">
         <v>5</v>
@@ -694,16 +694,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E12" s="1">
         <v>5</v>
@@ -714,13 +714,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E13" s="1">
         <v>500</v>
@@ -728,16 +728,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" s="1">
         <v>560</v>
@@ -748,13 +748,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="1">
         <f>ROUND(1/E8*1.1*1000,0)</f>
@@ -763,16 +763,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E16" s="1">
         <f>ROUND(1/E9*1.1*1000,0)</f>
@@ -784,13 +784,13 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="1">
         <v>5000</v>
@@ -798,16 +798,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="E18" s="1">
         <v>5500</v>
@@ -824,7 +824,7 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="1">
         <f>(1200-480)/2 + 480</f>
@@ -845,7 +845,7 @@
         <v>6</v>
       </c>
       <c r="D20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E20" s="1">
         <f>E19</f>
@@ -863,7 +863,7 @@
         <v>6</v>
       </c>
       <c r="D21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E21" s="1">
         <f>(3600-1700)/2 + 1700</f>
@@ -881,7 +881,7 @@
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E22" s="1">
         <f>(4300-3400)/2+3400</f>
@@ -890,7 +890,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23">
         <v>4</v>
@@ -899,7 +899,7 @@
         <v>6</v>
       </c>
       <c r="D23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E23" s="1">
         <f>(1200-480)/2 + 480</f>
@@ -920,7 +920,7 @@
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24" s="1">
         <f>E23</f>
@@ -929,7 +929,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25">
         <v>4</v>
@@ -938,7 +938,7 @@
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" s="1">
         <f>(3600-1700)/2 + 1700</f>
@@ -947,7 +947,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -956,7 +956,7 @@
         <v>6</v>
       </c>
       <c r="D26" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E26" s="1">
         <f>(4300-3400)/2+3400</f>
@@ -974,7 +974,7 @@
         <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E27" s="1">
         <f>(900-325)/2 + 325</f>
@@ -995,7 +995,7 @@
         <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E28" s="1">
         <f>E27</f>
@@ -1013,7 +1013,7 @@
         <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E29" s="1">
         <f>(2700-1300)/2 + 1300</f>
@@ -1031,7 +1031,7 @@
         <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E30" s="1">
         <f>(3300-2700)/2+2700</f>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31">
         <v>6</v>
@@ -1049,7 +1049,7 @@
         <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31" s="1">
         <f>(950-375)/2 + 375</f>
@@ -1070,7 +1070,7 @@
         <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E32" s="1">
         <f>E31</f>
@@ -1079,7 +1079,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33">
         <v>6</v>
@@ -1088,7 +1088,7 @@
         <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E33" s="1">
         <f>(3200-1500)/2 + 1500</f>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34">
         <v>6</v>
@@ -1106,7 +1106,7 @@
         <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E34" s="1">
         <f>(3500-3000)/2+3000</f>
@@ -1124,7 +1124,7 @@
         <v>14</v>
       </c>
       <c r="D35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E35" s="1">
         <f>(900-325)/2 + 325</f>
@@ -1145,7 +1145,7 @@
         <v>14</v>
       </c>
       <c r="D36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E36" s="1">
         <f>E35</f>
@@ -1163,7 +1163,7 @@
         <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E37" s="1">
         <f>(2700-1300)/2 + 1300</f>
@@ -1181,7 +1181,7 @@
         <v>14</v>
       </c>
       <c r="D38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E38" s="1">
         <f>(3300-2700)/2+2700</f>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39">
         <v>12</v>
@@ -1199,7 +1199,7 @@
         <v>14</v>
       </c>
       <c r="D39" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E39" s="1">
         <f>(950-375)/2 + 375</f>
@@ -1220,7 +1220,7 @@
         <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E40" s="1">
         <f>E39</f>
@@ -1229,7 +1229,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B41">
         <v>12</v>
@@ -1238,7 +1238,7 @@
         <v>14</v>
       </c>
       <c r="D41" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E41" s="1">
         <f>(3200-1500)/2 + 1500</f>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42">
         <v>12</v>
@@ -1256,7 +1256,7 @@
         <v>14</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E42" s="1">
         <f>(3500-3000)/2+3000</f>
@@ -1274,7 +1274,7 @@
         <v>16</v>
       </c>
       <c r="D43" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E43" s="1">
         <f>(850-325)/2 + 325</f>
@@ -1295,7 +1295,7 @@
         <v>16</v>
       </c>
       <c r="D44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E44" s="1">
         <f>E43</f>
@@ -1313,7 +1313,7 @@
         <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E45" s="1">
         <f>(2700-1300)/2 + 1300</f>
@@ -1331,7 +1331,7 @@
         <v>16</v>
       </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E46" s="1">
         <f>(3300-2700)/2+2700</f>
@@ -1340,7 +1340,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B47">
         <v>14</v>
@@ -1349,7 +1349,7 @@
         <v>16</v>
       </c>
       <c r="D47" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E47" s="1">
         <f>(900-400)/2 + 400</f>
@@ -1370,7 +1370,7 @@
         <v>16</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E48" s="1">
         <f>E47</f>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B49">
         <v>14</v>
@@ -1388,7 +1388,7 @@
         <v>16</v>
       </c>
       <c r="D49" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E49" s="1">
         <f>(2700-1600)/2 + 1600</f>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B50">
         <v>14</v>
@@ -1406,7 +1406,7 @@
         <v>16</v>
       </c>
       <c r="D50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E50" s="1">
         <f>(3300-2800)/2+2800</f>
@@ -1424,7 +1424,7 @@
         <v>18</v>
       </c>
       <c r="D51" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E51" s="1">
         <f>(750-300)/2 + 300</f>
@@ -1445,7 +1445,7 @@
         <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E52" s="1">
         <f>E51</f>
@@ -1463,7 +1463,7 @@
         <v>18</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E53" s="1">
         <f>(2300-1250)/2 + 1250</f>
@@ -1481,7 +1481,7 @@
         <v>18</v>
       </c>
       <c r="D54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E54" s="1">
         <f>(3000-2300)/2+2300</f>
@@ -1490,7 +1490,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B55">
         <v>16</v>
@@ -1499,7 +1499,7 @@
         <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E55" s="1">
         <f>(950-400)/2 + 400</f>
@@ -1520,7 +1520,7 @@
         <v>18</v>
       </c>
       <c r="D56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E56" s="1">
         <f>E55</f>
@@ -1529,7 +1529,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B57">
         <v>16</v>
@@ -1538,7 +1538,7 @@
         <v>18</v>
       </c>
       <c r="D57" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E57" s="1">
         <f>(2800-1800)/2 + 1800</f>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B58">
         <v>16</v>
@@ -1556,7 +1556,7 @@
         <v>18</v>
       </c>
       <c r="D58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E58" s="1">
         <f>(3300-2800)/2+2800</f>
@@ -1574,7 +1574,7 @@
         <v>18</v>
       </c>
       <c r="D59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E59" s="1">
         <f>(750-270)/2 + 270</f>
@@ -1595,7 +1595,7 @@
         <v>18</v>
       </c>
       <c r="D60" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E60" s="1">
         <f>E59</f>
@@ -1613,7 +1613,7 @@
         <v>18</v>
       </c>
       <c r="D61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E61" s="1">
         <f>(2300-900)/2 + 900</f>
@@ -1631,7 +1631,7 @@
         <v>18</v>
       </c>
       <c r="D62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E62" s="1">
         <f>(3000-2300)/2+2300</f>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B63">
         <v>18</v>
@@ -1649,7 +1649,7 @@
         <v>18</v>
       </c>
       <c r="D63" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E63" s="1">
         <f>(900-350)/2 + 350</f>
@@ -1670,7 +1670,7 @@
         <v>18</v>
       </c>
       <c r="D64" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E64" s="1">
         <f>E63</f>
@@ -1679,7 +1679,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B65">
         <v>18</v>
@@ -1688,7 +1688,7 @@
         <v>18</v>
       </c>
       <c r="D65" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E65" s="1">
         <f>(2800-1300)/2 + 1300</f>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B66">
         <v>18</v>
@@ -1706,7 +1706,7 @@
         <v>18</v>
       </c>
       <c r="D66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E66" s="1">
         <f>(3400-2700)/2+2700</f>
@@ -1724,7 +1724,7 @@
         <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E67" s="1">
         <v>199</v>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B68">
         <v>5</v>
@@ -1741,7 +1741,7 @@
         <v>10</v>
       </c>
       <c r="D68" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E68" s="1">
         <v>195</v>
@@ -1758,7 +1758,7 @@
         <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E69" s="1">
         <v>342</v>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B70">
         <v>5</v>
@@ -1775,7 +1775,7 @@
         <v>10</v>
       </c>
       <c r="D70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E70" s="1">
         <v>474</v>
@@ -1792,7 +1792,7 @@
         <v>30</v>
       </c>
       <c r="D71" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E71" s="1">
         <v>5200</v>
@@ -1800,7 +1800,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B72">
         <v>18</v>
@@ -1809,7 +1809,7 @@
         <v>30</v>
       </c>
       <c r="D72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E72" s="1">
         <v>6300</v>

</xml_diff>

<commit_message>
Implementation of a new metadata aware trackdata function is done, but largely untested at this point.
</commit_message>
<xml_diff>
--- a/inst/default_parameters.xlsx
+++ b/inst/default_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frkkan96/Documents/src/reindeer/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7FDE29B-BD82-9347-910F-8755C7568729}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEA2DBE-48F4-0F49-8550-396C2CAFA47B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25620" yWindow="500" windowWidth="25580" windowHeight="28300" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25580" windowHeight="28300" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="21">
   <si>
     <t>Gender</t>
   </si>
@@ -494,15 +494,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3287FC8-0847-0B47-A33C-7A45B3569376}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="209" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="207" zoomScaleNormal="207" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -711,7 +711,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -720,15 +720,15 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1">
-        <v>500</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -740,12 +740,12 @@
         <v>12</v>
       </c>
       <c r="E14" s="1">
-        <v>560</v>
+        <v>500</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -754,34 +754,33 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E16" s="1">
         <f>ROUND(1/E8*1.1*1000,0)</f>
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="1">
-        <f>ROUND(1/E9*1.1*1000,0)</f>
-        <v>14</v>
-      </c>
-    </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
@@ -790,15 +789,16 @@
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E17" s="1">
-        <v>5000</v>
+        <f>ROUND(1/E9*1.1*1000,0)</f>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -810,929 +810,929 @@
         <v>19</v>
       </c>
       <c r="E18" s="1">
-        <v>5500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
         <v>4</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="1">
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1">
         <f>(1200-480)/2 + 480</f>
         <v>840</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="str">
-        <f>A19</f>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="str">
+        <f>A20</f>
         <v>Male</v>
       </c>
-      <c r="B20">
-        <f>B19</f>
+      <c r="B21">
+        <f>B20</f>
         <v>4</v>
       </c>
-      <c r="C20">
-        <f>C19</f>
+      <c r="C21">
+        <f>C20</f>
         <v>6</v>
       </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="1">
-        <f>E19</f>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="1">
+        <f>E20</f>
         <v>840</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>1</v>
-      </c>
-      <c r="B21">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22">
         <v>4</v>
       </c>
-      <c r="C21">
+      <c r="C22">
         <v>6</v>
       </c>
-      <c r="D21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1">
         <f>(3600-1700)/2 + 1700</f>
         <v>2650</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23">
         <v>4</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>6</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E23" s="1">
         <f>(4300-3400)/2+3400</f>
         <v>3850</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
         <v>4</v>
       </c>
-      <c r="C23">
+      <c r="C24">
         <v>6</v>
       </c>
-      <c r="D23" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="1">
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="1">
         <f>(1200-480)/2 + 480</f>
         <v>840</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="str">
-        <f>A23</f>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="str">
+        <f>A24</f>
         <v>Female</v>
       </c>
-      <c r="B24">
-        <f>B23</f>
+      <c r="B25">
+        <f>B24</f>
         <v>4</v>
       </c>
-      <c r="C24">
-        <f>C23</f>
+      <c r="C25">
+        <f>C24</f>
         <v>6</v>
       </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="1">
-        <f>E23</f>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="1">
+        <f>E24</f>
         <v>840</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
         <v>4</v>
       </c>
-      <c r="C25">
+      <c r="C26">
         <v>6</v>
       </c>
-      <c r="D25" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="1">
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1">
         <f>(3600-1700)/2 + 1700</f>
         <v>2650</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
         <v>4</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>6</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E27" s="1">
         <f>(4300-3400)/2+3400</f>
         <v>3850</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28">
         <v>6</v>
       </c>
-      <c r="C27">
-        <v>12</v>
-      </c>
-      <c r="D27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="1">
+      <c r="C28">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="1">
         <f>(900-325)/2 + 325</f>
         <v>612.5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="str">
-        <f>A27</f>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="str">
+        <f>A28</f>
         <v>Male</v>
       </c>
-      <c r="B28">
-        <f>B27</f>
+      <c r="B29">
+        <f>B28</f>
         <v>6</v>
       </c>
-      <c r="C28">
-        <f>C27</f>
-        <v>12</v>
-      </c>
-      <c r="D28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="1">
-        <f>E27</f>
+      <c r="C29">
+        <f>C28</f>
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="1">
+        <f>E28</f>
         <v>612.5</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="B29">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30">
         <v>6</v>
       </c>
-      <c r="C29">
-        <v>12</v>
-      </c>
-      <c r="D29" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="1">
+      <c r="C30">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="1">
         <f>(2700-1300)/2 + 1300</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31">
         <v>6</v>
       </c>
-      <c r="C30">
-        <v>12</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C31">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E31" s="1">
         <f>(3300-2700)/2+2700</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32">
         <v>6</v>
       </c>
-      <c r="C31">
-        <v>12</v>
-      </c>
-      <c r="D31" t="s">
-        <v>14</v>
-      </c>
-      <c r="E31" s="1">
+      <c r="C32">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="1">
         <f>(950-375)/2 + 375</f>
         <v>662.5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="str">
-        <f>A31</f>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="str">
+        <f>A32</f>
         <v>Female</v>
       </c>
-      <c r="B32">
-        <f>B31</f>
+      <c r="B33">
+        <f>B32</f>
         <v>6</v>
       </c>
-      <c r="C32">
-        <f>C31</f>
-        <v>12</v>
-      </c>
-      <c r="D32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="1">
-        <f>E31</f>
+      <c r="C33">
+        <f>C32</f>
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="1">
+        <f>E32</f>
         <v>662.5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34">
         <v>6</v>
       </c>
-      <c r="C33">
-        <v>12</v>
-      </c>
-      <c r="D33" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="1">
+      <c r="C34">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="1">
         <f>(3200-1500)/2 + 1500</f>
         <v>2350</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35">
         <v>6</v>
       </c>
-      <c r="C34">
-        <v>12</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="C35">
+        <v>12</v>
+      </c>
+      <c r="D35" t="s">
         <v>15</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E35" s="1">
         <f>(3500-3000)/2+3000</f>
         <v>3250</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35">
-        <v>12</v>
-      </c>
-      <c r="C35">
-        <v>14</v>
-      </c>
-      <c r="D35" t="s">
-        <v>14</v>
-      </c>
-      <c r="E35" s="1">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>14</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="1">
         <f>(900-325)/2 + 325</f>
         <v>612.5</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="str">
-        <f>A35</f>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="str">
+        <f>A36</f>
         <v>Male</v>
       </c>
-      <c r="B36">
-        <f>B35</f>
-        <v>12</v>
-      </c>
-      <c r="C36">
-        <f>C35</f>
-        <v>14</v>
-      </c>
-      <c r="D36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E36" s="1">
-        <f>E35</f>
+      <c r="B37">
+        <f>B36</f>
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <f>C36</f>
+        <v>14</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="1">
+        <f>E36</f>
         <v>612.5</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37">
-        <v>12</v>
-      </c>
-      <c r="C37">
-        <v>14</v>
-      </c>
-      <c r="D37" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="1">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>16</v>
+      </c>
+      <c r="E38" s="1">
         <f>(2700-1300)/2 + 1300</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38">
-        <v>12</v>
-      </c>
-      <c r="C38">
-        <v>14</v>
-      </c>
-      <c r="D38" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>14</v>
+      </c>
+      <c r="D39" t="s">
         <v>15</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E39" s="1">
         <f>(3300-2700)/2+2700</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>5</v>
-      </c>
-      <c r="B39">
-        <v>12</v>
-      </c>
-      <c r="C39">
-        <v>14</v>
-      </c>
-      <c r="D39" t="s">
-        <v>14</v>
-      </c>
-      <c r="E39" s="1">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="1">
         <f>(950-375)/2 + 375</f>
         <v>662.5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="str">
-        <f>A39</f>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="str">
+        <f>A40</f>
         <v>Female</v>
       </c>
-      <c r="B40">
-        <f>B39</f>
-        <v>12</v>
-      </c>
-      <c r="C40">
-        <f>C39</f>
-        <v>14</v>
-      </c>
-      <c r="D40" t="s">
-        <v>12</v>
-      </c>
-      <c r="E40" s="1">
-        <f>E39</f>
+      <c r="B41">
+        <f>B40</f>
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <f>C40</f>
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="1">
+        <f>E40</f>
         <v>662.5</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B41">
-        <v>12</v>
-      </c>
-      <c r="C41">
-        <v>14</v>
-      </c>
-      <c r="D41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="1">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>12</v>
+      </c>
+      <c r="C42">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
+      </c>
+      <c r="E42" s="1">
         <f>(3200-1500)/2 + 1500</f>
         <v>2350</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>5</v>
-      </c>
-      <c r="B42">
-        <v>12</v>
-      </c>
-      <c r="C42">
-        <v>14</v>
-      </c>
-      <c r="D42" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43">
+        <v>12</v>
+      </c>
+      <c r="C43">
+        <v>14</v>
+      </c>
+      <c r="D43" t="s">
         <v>15</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E43" s="1">
         <f>(3500-3000)/2+3000</f>
         <v>3250</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43">
-        <v>14</v>
-      </c>
-      <c r="C43">
-        <v>16</v>
-      </c>
-      <c r="D43" t="s">
-        <v>14</v>
-      </c>
-      <c r="E43" s="1">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>14</v>
+      </c>
+      <c r="C44">
+        <v>16</v>
+      </c>
+      <c r="D44" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="1">
         <f>(850-325)/2 + 325</f>
         <v>587.5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="str">
-        <f>A43</f>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="str">
+        <f>A44</f>
         <v>Male</v>
       </c>
-      <c r="B44">
-        <f>B43</f>
-        <v>14</v>
-      </c>
-      <c r="C44">
-        <f>C43</f>
-        <v>16</v>
-      </c>
-      <c r="D44" t="s">
-        <v>12</v>
-      </c>
-      <c r="E44" s="1">
-        <f>E43</f>
+      <c r="B45">
+        <f>B44</f>
+        <v>14</v>
+      </c>
+      <c r="C45">
+        <f>C44</f>
+        <v>16</v>
+      </c>
+      <c r="D45" t="s">
+        <v>12</v>
+      </c>
+      <c r="E45" s="1">
+        <f>E44</f>
         <v>587.5</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45">
-        <v>14</v>
-      </c>
-      <c r="C45">
-        <v>16</v>
-      </c>
-      <c r="D45" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="1">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>14</v>
+      </c>
+      <c r="C46">
+        <v>16</v>
+      </c>
+      <c r="D46" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="1">
         <f>(2700-1300)/2 + 1300</f>
         <v>2000</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46">
-        <v>14</v>
-      </c>
-      <c r="C46">
-        <v>16</v>
-      </c>
-      <c r="D46" t="s">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>14</v>
+      </c>
+      <c r="C47">
+        <v>16</v>
+      </c>
+      <c r="D47" t="s">
         <v>15</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E47" s="1">
         <f>(3300-2700)/2+2700</f>
         <v>3000</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47">
-        <v>14</v>
-      </c>
-      <c r="C47">
-        <v>16</v>
-      </c>
-      <c r="D47" t="s">
-        <v>14</v>
-      </c>
-      <c r="E47" s="1">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48">
+        <v>14</v>
+      </c>
+      <c r="C48">
+        <v>16</v>
+      </c>
+      <c r="D48" t="s">
+        <v>14</v>
+      </c>
+      <c r="E48" s="1">
         <f>(900-400)/2 + 400</f>
         <v>650</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48" t="str">
-        <f>A47</f>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="str">
+        <f>A48</f>
         <v>Female</v>
       </c>
-      <c r="B48">
-        <f>B47</f>
-        <v>14</v>
-      </c>
-      <c r="C48">
-        <f>C47</f>
-        <v>16</v>
-      </c>
-      <c r="D48" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="1">
-        <f>E47</f>
+      <c r="B49">
+        <f>B48</f>
+        <v>14</v>
+      </c>
+      <c r="C49">
+        <f>C48</f>
+        <v>16</v>
+      </c>
+      <c r="D49" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="1">
+        <f>E48</f>
         <v>650</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49">
-        <v>14</v>
-      </c>
-      <c r="C49">
-        <v>16</v>
-      </c>
-      <c r="D49" t="s">
-        <v>16</v>
-      </c>
-      <c r="E49" s="1">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50">
+        <v>14</v>
+      </c>
+      <c r="C50">
+        <v>16</v>
+      </c>
+      <c r="D50" t="s">
+        <v>16</v>
+      </c>
+      <c r="E50" s="1">
         <f>(2700-1600)/2 + 1600</f>
         <v>2150</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50">
-        <v>14</v>
-      </c>
-      <c r="C50">
-        <v>16</v>
-      </c>
-      <c r="D50" t="s">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51">
+        <v>14</v>
+      </c>
+      <c r="C51">
+        <v>16</v>
+      </c>
+      <c r="D51" t="s">
         <v>15</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E51" s="1">
         <f>(3300-2800)/2+2800</f>
         <v>3050</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>1</v>
-      </c>
-      <c r="B51">
-        <v>16</v>
-      </c>
-      <c r="C51">
-        <v>18</v>
-      </c>
-      <c r="D51" t="s">
-        <v>14</v>
-      </c>
-      <c r="E51" s="1">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>16</v>
+      </c>
+      <c r="C52">
+        <v>18</v>
+      </c>
+      <c r="D52" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" s="1">
         <f>(750-300)/2 + 300</f>
         <v>525</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52" t="str">
-        <f>A51</f>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" t="str">
+        <f>A52</f>
         <v>Male</v>
       </c>
-      <c r="B52">
-        <f>B51</f>
-        <v>16</v>
-      </c>
-      <c r="C52">
-        <f>C51</f>
-        <v>18</v>
-      </c>
-      <c r="D52" t="s">
-        <v>12</v>
-      </c>
-      <c r="E52" s="1">
-        <f>E51</f>
+      <c r="B53">
+        <f>B52</f>
+        <v>16</v>
+      </c>
+      <c r="C53">
+        <f>C52</f>
+        <v>18</v>
+      </c>
+      <c r="D53" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="1">
+        <f>E52</f>
         <v>525</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53" t="s">
-        <v>1</v>
-      </c>
-      <c r="B53">
-        <v>16</v>
-      </c>
-      <c r="C53">
-        <v>18</v>
-      </c>
-      <c r="D53" t="s">
-        <v>16</v>
-      </c>
-      <c r="E53" s="1">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>16</v>
+      </c>
+      <c r="C54">
+        <v>18</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="1">
         <f>(2300-1250)/2 + 1250</f>
         <v>1775</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B54">
-        <v>16</v>
-      </c>
-      <c r="C54">
-        <v>18</v>
-      </c>
-      <c r="D54" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>16</v>
+      </c>
+      <c r="C55">
+        <v>18</v>
+      </c>
+      <c r="D55" t="s">
         <v>15</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E55" s="1">
         <f>(3000-2300)/2+2300</f>
         <v>2650</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>5</v>
-      </c>
-      <c r="B55">
-        <v>16</v>
-      </c>
-      <c r="C55">
-        <v>18</v>
-      </c>
-      <c r="D55" t="s">
-        <v>14</v>
-      </c>
-      <c r="E55" s="1">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>16</v>
+      </c>
+      <c r="C56">
+        <v>18</v>
+      </c>
+      <c r="D56" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="1">
         <f>(950-400)/2 + 400</f>
         <v>675</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" t="str">
-        <f>A55</f>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" t="str">
+        <f>A56</f>
         <v>Female</v>
       </c>
-      <c r="B56">
-        <f>B55</f>
-        <v>16</v>
-      </c>
-      <c r="C56">
-        <f>C55</f>
-        <v>18</v>
-      </c>
-      <c r="D56" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56" s="1">
-        <f>E55</f>
+      <c r="B57">
+        <f>B56</f>
+        <v>16</v>
+      </c>
+      <c r="C57">
+        <f>C56</f>
+        <v>18</v>
+      </c>
+      <c r="D57" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" s="1">
+        <f>E56</f>
         <v>675</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57">
-        <v>16</v>
-      </c>
-      <c r="C57">
-        <v>18</v>
-      </c>
-      <c r="D57" t="s">
-        <v>16</v>
-      </c>
-      <c r="E57" s="1">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58">
+        <v>16</v>
+      </c>
+      <c r="C58">
+        <v>18</v>
+      </c>
+      <c r="D58" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" s="1">
         <f>(2800-1800)/2 + 1800</f>
         <v>2300</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58">
-        <v>16</v>
-      </c>
-      <c r="C58">
-        <v>18</v>
-      </c>
-      <c r="D58" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>16</v>
+      </c>
+      <c r="C59">
+        <v>18</v>
+      </c>
+      <c r="D59" t="s">
         <v>15</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E59" s="1">
         <f>(3300-2800)/2+2800</f>
         <v>3050</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>1</v>
-      </c>
-      <c r="B59">
-        <v>18</v>
-      </c>
-      <c r="C59">
-        <v>18</v>
-      </c>
-      <c r="D59" t="s">
-        <v>14</v>
-      </c>
-      <c r="E59" s="1">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>18</v>
+      </c>
+      <c r="C60">
+        <v>18</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+      <c r="E60" s="1">
         <f>(750-270)/2 + 270</f>
         <v>510</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" t="str">
-        <f>A59</f>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" t="str">
+        <f>A60</f>
         <v>Male</v>
       </c>
-      <c r="B60">
-        <f>B59</f>
-        <v>18</v>
-      </c>
-      <c r="C60">
-        <f>C59</f>
-        <v>18</v>
-      </c>
-      <c r="D60" t="s">
-        <v>12</v>
-      </c>
-      <c r="E60" s="1">
-        <f>E59</f>
+      <c r="B61">
+        <f>B60</f>
+        <v>18</v>
+      </c>
+      <c r="C61">
+        <f>C60</f>
+        <v>18</v>
+      </c>
+      <c r="D61" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="1">
+        <f>E60</f>
         <v>510</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>1</v>
-      </c>
-      <c r="B61">
-        <v>18</v>
-      </c>
-      <c r="C61">
-        <v>18</v>
-      </c>
-      <c r="D61" t="s">
-        <v>16</v>
-      </c>
-      <c r="E61" s="1">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>18</v>
+      </c>
+      <c r="C62">
+        <v>18</v>
+      </c>
+      <c r="D62" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="1">
         <f>(2300-900)/2 + 900</f>
         <v>1600</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>1</v>
-      </c>
-      <c r="B62">
-        <v>18</v>
-      </c>
-      <c r="C62">
-        <v>18</v>
-      </c>
-      <c r="D62" t="s">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>18</v>
+      </c>
+      <c r="C63">
+        <v>18</v>
+      </c>
+      <c r="D63" t="s">
         <v>15</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E63" s="1">
         <f>(3000-2300)/2+2300</f>
         <v>2650</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>5</v>
-      </c>
-      <c r="B63">
-        <v>18</v>
-      </c>
-      <c r="C63">
-        <v>18</v>
-      </c>
-      <c r="D63" t="s">
-        <v>14</v>
-      </c>
-      <c r="E63" s="1">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64">
+        <v>18</v>
+      </c>
+      <c r="C64">
+        <v>18</v>
+      </c>
+      <c r="D64" t="s">
+        <v>14</v>
+      </c>
+      <c r="E64" s="1">
         <f>(900-350)/2 + 350</f>
         <v>625</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" t="str">
-        <f>A63</f>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" t="str">
+        <f>A64</f>
         <v>Female</v>
       </c>
-      <c r="B64">
-        <f>B63</f>
-        <v>18</v>
-      </c>
-      <c r="C64">
-        <f>C63</f>
-        <v>18</v>
-      </c>
-      <c r="D64" t="s">
-        <v>12</v>
-      </c>
-      <c r="E64" s="1">
-        <f>E63</f>
+      <c r="B65">
+        <f>B64</f>
+        <v>18</v>
+      </c>
+      <c r="C65">
+        <f>C64</f>
+        <v>18</v>
+      </c>
+      <c r="D65" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" s="1">
+        <f>E64</f>
         <v>625</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>5</v>
-      </c>
-      <c r="B65">
-        <v>18</v>
-      </c>
-      <c r="C65">
-        <v>18</v>
-      </c>
-      <c r="D65" t="s">
-        <v>16</v>
-      </c>
-      <c r="E65" s="1">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66">
+        <v>18</v>
+      </c>
+      <c r="C66">
+        <v>18</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" s="1">
         <f>(2800-1300)/2 + 1300</f>
         <v>2050</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>5</v>
-      </c>
-      <c r="B66">
-        <v>18</v>
-      </c>
-      <c r="C66">
-        <v>18</v>
-      </c>
-      <c r="D66" t="s">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>5</v>
+      </c>
+      <c r="B67">
+        <v>18</v>
+      </c>
+      <c r="C67">
+        <v>18</v>
+      </c>
+      <c r="D67" t="s">
         <v>15</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E67" s="1">
         <f>(3400-2700)/2+2700</f>
         <v>3050</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67">
-        <v>5</v>
-      </c>
-      <c r="C67">
-        <v>10</v>
-      </c>
-      <c r="D67" t="s">
-        <v>10</v>
-      </c>
-      <c r="E67" s="1">
-        <v>199</v>
-      </c>
-    </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B68">
         <v>5</v>
@@ -1744,12 +1744,12 @@
         <v>10</v>
       </c>
       <c r="E68" s="1">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B69">
         <v>5</v>
@@ -1758,15 +1758,15 @@
         <v>10</v>
       </c>
       <c r="D69" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E69" s="1">
-        <v>342</v>
+        <v>195</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B70">
         <v>5</v>
@@ -1778,29 +1778,29 @@
         <v>9</v>
       </c>
       <c r="E70" s="1">
-        <v>474</v>
+        <v>342</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B71">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C71">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D71" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E71" s="1">
-        <v>5200</v>
+        <v>474</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B72">
         <v>18</v>
@@ -1809,9 +1809,26 @@
         <v>30</v>
       </c>
       <c r="D72" t="s">
+        <v>19</v>
+      </c>
+      <c r="E72" s="1">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73">
+        <v>18</v>
+      </c>
+      <c r="C73">
+        <v>30</v>
+      </c>
+      <c r="D73" t="s">
         <v>13</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E73" s="1">
         <v>6300</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed erroneous windowSize defaults for women.
</commit_message>
<xml_diff>
--- a/inst/default_parameters.xlsx
+++ b/inst/default_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frkkan96/Documents/src/reindeer/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75CD1F2-577C-0A45-9E39-905D5640CDF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCB543C-D75B-674E-9F85-AFC42CD77CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24920" yWindow="500" windowWidth="25580" windowHeight="28300" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
+    <workbookView xWindow="24920" yWindow="500" windowWidth="42200" windowHeight="39900" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3287FC8-0847-0B47-A33C-7A45B3569376}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53:D55"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1571,7 +1571,7 @@
         <v>30</v>
       </c>
       <c r="D61" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E61" s="1">
         <v>6300</v>

</xml_diff>

<commit_message>
Revised formant frequency defaults from 10.1121/1.426686
</commit_message>
<xml_diff>
--- a/inst/default_parameters.xlsx
+++ b/inst/default_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frkkan96/Documents/src/reindeer/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF80C3AF-7DAD-0141-8E8E-ECDFCB2058F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC869E2-C02F-854C-96E2-F4A53B95EDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35460" yWindow="1360" windowWidth="38380" windowHeight="21320" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -188,7 +188,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -217,12 +217,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -588,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3287FC8-0847-0B47-A33C-7A45B3569376}">
   <dimension ref="A1:G260"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2672,7 +2666,7 @@
         <v>12</v>
       </c>
       <c r="E89" s="1">
-        <v>752.8</v>
+        <v>816.5</v>
       </c>
       <c r="F89" s="1">
         <v>19</v>
@@ -2695,7 +2689,7 @@
         <v>18</v>
       </c>
       <c r="E90" s="1">
-        <v>1998</v>
+        <v>2148.5</v>
       </c>
       <c r="F90" s="1">
         <v>19</v>
@@ -2718,7 +2712,7 @@
         <v>17</v>
       </c>
       <c r="E91" s="1">
-        <v>3380.6</v>
+        <v>3077.5</v>
       </c>
       <c r="F91" s="1">
         <v>19</v>
@@ -2742,7 +2736,7 @@
         <v>12</v>
       </c>
       <c r="E92" s="1">
-        <v>739.9</v>
+        <v>729.5</v>
       </c>
       <c r="F92" s="1">
         <v>11</v>
@@ -2767,7 +2761,7 @@
         <v>18</v>
       </c>
       <c r="E93" s="1">
-        <v>1972.4</v>
+        <v>2135.5</v>
       </c>
       <c r="F93" s="1">
         <f>F92</f>
@@ -2793,7 +2787,7 @@
         <v>17</v>
       </c>
       <c r="E94" s="1">
-        <v>3326.8</v>
+        <v>2930</v>
       </c>
       <c r="F94" s="1">
         <f>F92</f>
@@ -2819,7 +2813,7 @@
         <v>12</v>
       </c>
       <c r="E95" s="1">
-        <v>699.8</v>
+        <v>704.5</v>
       </c>
       <c r="F95" s="1">
         <v>11</v>
@@ -2844,7 +2838,7 @@
         <v>18</v>
       </c>
       <c r="E96" s="1">
-        <v>1973.7</v>
+        <v>2112.5</v>
       </c>
       <c r="F96" s="1">
         <f>F95</f>
@@ -2870,7 +2864,7 @@
         <v>17</v>
       </c>
       <c r="E97" s="1">
-        <v>3289.8</v>
+        <v>2935.5</v>
       </c>
       <c r="F97" s="1">
         <f>F95</f>
@@ -2896,7 +2890,7 @@
         <v>12</v>
       </c>
       <c r="E98" s="1">
-        <v>676.9</v>
+        <v>691.5</v>
       </c>
       <c r="F98" s="1">
         <v>25</v>
@@ -2921,7 +2915,7 @@
         <v>18</v>
       </c>
       <c r="E99" s="1">
-        <v>1925.7</v>
+        <v>2106</v>
       </c>
       <c r="F99" s="1">
         <f>F98</f>
@@ -2947,7 +2941,7 @@
         <v>17</v>
       </c>
       <c r="E100" s="1">
-        <v>3241.8</v>
+        <v>2919</v>
       </c>
       <c r="F100" s="1">
         <f>F98</f>
@@ -2973,7 +2967,7 @@
         <v>12</v>
       </c>
       <c r="E101" s="1">
-        <v>690.9</v>
+        <v>696.5</v>
       </c>
       <c r="F101" s="4">
         <v>23</v>
@@ -2998,7 +2992,7 @@
         <v>18</v>
       </c>
       <c r="E102" s="1">
-        <v>1905.9</v>
+        <v>2074.5</v>
       </c>
       <c r="F102" s="4">
         <f>F101</f>
@@ -3024,7 +3018,7 @@
         <v>17</v>
       </c>
       <c r="E103" s="1">
-        <v>3224.1</v>
+        <v>2820</v>
       </c>
       <c r="F103" s="4">
         <f>F101</f>
@@ -3050,7 +3044,7 @@
         <v>12</v>
       </c>
       <c r="E104" s="1">
-        <v>687.9</v>
+        <v>697</v>
       </c>
       <c r="F104" s="1">
         <v>25</v>
@@ -3075,7 +3069,7 @@
         <v>18</v>
       </c>
       <c r="E105" s="1">
-        <v>1903.2</v>
+        <v>2060.5</v>
       </c>
       <c r="F105" s="1">
         <v>25</v>
@@ -3100,7 +3094,7 @@
         <v>17</v>
       </c>
       <c r="E106" s="1">
-        <v>3168</v>
+        <v>2822.5</v>
       </c>
       <c r="F106" s="1">
         <v>25</v>
@@ -3125,7 +3119,7 @@
         <v>12</v>
       </c>
       <c r="E107" s="1">
-        <v>656.1</v>
+        <v>650</v>
       </c>
       <c r="F107" s="1">
         <v>24</v>
@@ -3150,7 +3144,7 @@
         <v>18</v>
       </c>
       <c r="E108" s="1">
-        <v>1837.5</v>
+        <v>1990</v>
       </c>
       <c r="F108" s="1">
         <v>24</v>
@@ -3175,7 +3169,7 @@
         <v>17</v>
       </c>
       <c r="E109" s="1">
-        <v>3045.8</v>
+        <v>2725</v>
       </c>
       <c r="F109" s="1">
         <v>24</v>
@@ -3200,7 +3194,7 @@
         <v>12</v>
       </c>
       <c r="E110" s="1">
-        <v>631.1</v>
+        <v>624.5</v>
       </c>
       <c r="F110" s="1">
         <v>22</v>
@@ -3225,7 +3219,7 @@
         <v>18</v>
       </c>
       <c r="E111" s="1">
-        <v>1763.3</v>
+        <v>1919</v>
       </c>
       <c r="F111" s="1">
         <v>22</v>
@@ -3250,7 +3244,7 @@
         <v>17</v>
       </c>
       <c r="E112" s="1">
-        <v>2965.8</v>
+        <v>2678</v>
       </c>
       <c r="F112" s="1">
         <v>22</v>
@@ -3275,7 +3269,7 @@
         <v>12</v>
       </c>
       <c r="E113" s="1">
-        <v>588.5</v>
+        <v>576.5</v>
       </c>
       <c r="F113" s="1">
         <v>16</v>
@@ -3300,7 +3294,7 @@
         <v>18</v>
       </c>
       <c r="E114" s="1">
-        <v>1642.2</v>
+        <v>1777.5</v>
       </c>
       <c r="F114" s="1">
         <v>16</v>
@@ -3325,7 +3319,7 @@
         <v>17</v>
       </c>
       <c r="E115" s="1">
-        <v>2754.6</v>
+        <v>2568.5</v>
       </c>
       <c r="F115" s="1">
         <v>16</v>
@@ -3350,7 +3344,7 @@
         <v>12</v>
       </c>
       <c r="E116" s="1">
-        <v>595.9</v>
+        <v>597</v>
       </c>
       <c r="F116" s="1">
         <v>11</v>
@@ -3375,7 +3369,7 @@
         <v>18</v>
       </c>
       <c r="E117" s="1">
-        <v>1700.3</v>
+        <v>1861.5</v>
       </c>
       <c r="F117" s="1">
         <v>11</v>
@@ -3400,7 +3394,7 @@
         <v>17</v>
       </c>
       <c r="E118" s="1">
-        <v>2784.5</v>
+        <v>2607</v>
       </c>
       <c r="F118" s="1">
         <v>11</v>
@@ -3425,7 +3419,7 @@
         <v>12</v>
       </c>
       <c r="E119" s="1">
-        <v>538.20000000000005</v>
+        <v>520.5</v>
       </c>
       <c r="F119" s="1">
         <v>11</v>
@@ -3450,7 +3444,7 @@
         <v>18</v>
       </c>
       <c r="E120" s="1">
-        <v>1545.5</v>
+        <v>1663</v>
       </c>
       <c r="F120" s="1">
         <v>11</v>
@@ -3475,7 +3469,7 @@
         <v>17</v>
       </c>
       <c r="E121" s="1">
-        <v>2548.4</v>
+        <v>2359.5</v>
       </c>
       <c r="F121" s="1">
         <v>11</v>
@@ -3500,7 +3494,7 @@
         <v>12</v>
       </c>
       <c r="E122" s="1">
-        <v>497</v>
+        <v>387.5</v>
       </c>
       <c r="F122" s="1">
         <v>11</v>
@@ -3525,7 +3519,7 @@
         <v>18</v>
       </c>
       <c r="E123" s="1">
-        <v>1527.4</v>
+        <v>1634.5</v>
       </c>
       <c r="F123" s="1">
         <v>11</v>
@@ -3550,7 +3544,7 @@
         <v>17</v>
       </c>
       <c r="E124" s="1">
-        <v>2589.4</v>
+        <v>2392</v>
       </c>
       <c r="F124" s="1">
         <v>11</v>
@@ -3575,7 +3569,7 @@
         <v>12</v>
       </c>
       <c r="E125" s="1">
-        <v>524.9</v>
+        <v>501</v>
       </c>
       <c r="F125" s="1">
         <v>10</v>
@@ -3600,7 +3594,7 @@
         <v>18</v>
       </c>
       <c r="E126" s="1">
-        <v>1503.2</v>
+        <v>1604</v>
       </c>
       <c r="F126" s="1">
         <v>10</v>
@@ -3625,7 +3619,7 @@
         <v>17</v>
       </c>
       <c r="E127" s="1">
-        <v>2567.9</v>
+        <v>2398</v>
       </c>
       <c r="F127" s="1">
         <v>10</v>
@@ -3650,7 +3644,7 @@
         <v>12</v>
       </c>
       <c r="E128" s="1">
-        <v>532</v>
+        <v>510</v>
       </c>
       <c r="F128" s="1">
         <v>10</v>
@@ -3675,7 +3669,7 @@
         <v>18</v>
       </c>
       <c r="E129" s="1">
-        <v>1490.4</v>
+        <v>1585</v>
       </c>
       <c r="F129" s="1">
         <v>10</v>
@@ -3700,7 +3694,7 @@
         <v>17</v>
       </c>
       <c r="E130" s="1">
-        <v>2525.6</v>
+        <v>2337.5</v>
       </c>
       <c r="F130" s="1">
         <v>10</v>
@@ -3723,7 +3717,7 @@
         <v>12</v>
       </c>
       <c r="E131" s="1">
-        <v>525.70000000000005</v>
+        <v>507.5</v>
       </c>
       <c r="F131" s="1">
         <v>29</v>
@@ -3746,7 +3740,7 @@
         <v>18</v>
       </c>
       <c r="E132" s="1">
-        <v>1468.9</v>
+        <v>1597.5</v>
       </c>
       <c r="F132" s="1">
         <v>29</v>
@@ -3769,7 +3763,7 @@
         <v>17</v>
       </c>
       <c r="E133" s="1">
-        <v>2474</v>
+        <v>2271</v>
       </c>
       <c r="F133" s="1">
         <v>29</v>
@@ -3792,7 +3786,7 @@
         <v>12</v>
       </c>
       <c r="E134" s="1">
-        <v>808.7</v>
+        <v>845</v>
       </c>
       <c r="F134" s="1">
         <v>13</v>
@@ -3815,7 +3809,7 @@
         <v>18</v>
       </c>
       <c r="E135" s="1">
-        <v>2074.6</v>
+        <v>2178</v>
       </c>
       <c r="F135" s="1">
         <v>13</v>
@@ -3838,7 +3832,7 @@
         <v>17</v>
       </c>
       <c r="E136" s="1">
-        <v>3330.7</v>
+        <v>3012.5</v>
       </c>
       <c r="F136" s="1">
         <v>13</v>
@@ -3862,7 +3856,7 @@
         <v>12</v>
       </c>
       <c r="E137" s="1">
-        <v>755.8</v>
+        <v>798</v>
       </c>
       <c r="F137" s="1">
         <v>16</v>
@@ -3887,7 +3881,7 @@
         <v>18</v>
       </c>
       <c r="E138" s="1">
-        <v>2109</v>
+        <v>2122</v>
       </c>
       <c r="F138" s="1">
         <v>16</v>
@@ -3912,7 +3906,7 @@
         <v>17</v>
       </c>
       <c r="E139" s="1">
-        <v>3433.4</v>
+        <v>3108.5</v>
       </c>
       <c r="F139" s="1">
         <v>16</v>
@@ -3937,7 +3931,7 @@
         <v>12</v>
       </c>
       <c r="E140" s="1">
-        <v>757.3</v>
+        <v>767</v>
       </c>
       <c r="F140" s="1">
         <v>24</v>
@@ -3962,7 +3956,7 @@
         <v>18</v>
       </c>
       <c r="E141" s="1">
-        <v>2032.4</v>
+        <v>2152.5</v>
       </c>
       <c r="F141" s="1">
         <v>24</v>
@@ -3987,7 +3981,7 @@
         <v>17</v>
       </c>
       <c r="E142" s="1">
-        <v>3354.3</v>
+        <v>3031.5</v>
       </c>
       <c r="F142" s="1">
         <v>24</v>
@@ -4012,7 +4006,7 @@
         <v>12</v>
       </c>
       <c r="E143" s="1">
-        <v>739.6</v>
+        <v>767</v>
       </c>
       <c r="F143" s="1">
         <v>11</v>
@@ -4037,7 +4031,7 @@
         <v>18</v>
       </c>
       <c r="E144" s="1">
-        <v>1978.2</v>
+        <v>2135.5</v>
       </c>
       <c r="F144" s="1">
         <v>11</v>
@@ -4062,7 +4056,7 @@
         <v>17</v>
       </c>
       <c r="E145" s="1">
-        <v>3299.1</v>
+        <v>2992.5</v>
       </c>
       <c r="F145" s="1">
         <v>11</v>
@@ -4087,7 +4081,7 @@
         <v>12</v>
       </c>
       <c r="E146" s="1">
-        <v>728.2</v>
+        <v>759</v>
       </c>
       <c r="F146" s="1">
         <v>25</v>
@@ -4112,7 +4106,7 @@
         <v>18</v>
       </c>
       <c r="E147" s="1">
-        <v>2000.9</v>
+        <v>2155.5</v>
       </c>
       <c r="F147" s="1">
         <v>25</v>
@@ -4137,7 +4131,7 @@
         <v>17</v>
       </c>
       <c r="E148" s="1">
-        <v>3303.6</v>
+        <v>2962</v>
       </c>
       <c r="F148" s="1">
         <v>25</v>
@@ -4162,7 +4156,7 @@
         <v>12</v>
       </c>
       <c r="E149" s="1">
-        <v>730.5</v>
+        <v>754.5</v>
       </c>
       <c r="F149" s="1">
         <v>14</v>
@@ -4187,7 +4181,7 @@
         <v>18</v>
       </c>
       <c r="E150" s="1">
-        <v>1992.8</v>
+        <v>2116.5</v>
       </c>
       <c r="F150" s="1">
         <v>14</v>
@@ -4212,7 +4206,7 @@
         <v>17</v>
       </c>
       <c r="E151" s="1">
-        <v>3238.3</v>
+        <v>2885</v>
       </c>
       <c r="F151" s="1">
         <v>14</v>
@@ -4237,7 +4231,7 @@
         <v>12</v>
       </c>
       <c r="E152" s="1">
-        <v>699.6</v>
+        <v>723.5</v>
       </c>
       <c r="F152" s="1">
         <v>19</v>
@@ -4262,7 +4256,7 @@
         <v>18</v>
       </c>
       <c r="E153" s="1">
-        <v>1930.4</v>
+        <v>2095</v>
       </c>
       <c r="F153" s="1">
         <v>19</v>
@@ -4287,7 +4281,7 @@
         <v>17</v>
       </c>
       <c r="E154" s="1">
-        <v>3151.8</v>
+        <v>2814.5</v>
       </c>
       <c r="F154" s="1">
         <v>19</v>
@@ -4312,7 +4306,7 @@
         <v>12</v>
       </c>
       <c r="E155" s="1">
-        <v>662.9</v>
+        <v>689</v>
       </c>
       <c r="F155" s="1">
         <v>21</v>
@@ -4337,7 +4331,7 @@
         <v>18</v>
       </c>
       <c r="E156" s="1">
-        <v>1910.5</v>
+        <v>2048</v>
       </c>
       <c r="F156" s="1">
         <v>21</v>
@@ -4362,7 +4356,7 @@
         <v>17</v>
       </c>
       <c r="E157" s="1">
-        <v>3096.9</v>
+        <v>2811.5</v>
       </c>
       <c r="F157" s="1">
         <v>21</v>
@@ -4387,7 +4381,7 @@
         <v>12</v>
       </c>
       <c r="E158" s="1">
-        <v>687.4</v>
+        <v>692.5</v>
       </c>
       <c r="F158" s="1">
         <v>13</v>
@@ -4412,7 +4406,7 @@
         <v>18</v>
       </c>
       <c r="E159" s="1">
-        <v>1919.1</v>
+        <v>2036.5</v>
       </c>
       <c r="F159" s="1">
         <v>13</v>
@@ -4437,7 +4431,7 @@
         <v>17</v>
       </c>
       <c r="E160" s="1">
-        <v>3075.9</v>
+        <v>2776</v>
       </c>
       <c r="F160" s="1">
         <v>13</v>
@@ -4462,7 +4456,7 @@
         <v>12</v>
       </c>
       <c r="E161" s="1">
-        <v>663.3</v>
+        <v>654</v>
       </c>
       <c r="F161" s="1">
         <v>10</v>
@@ -4487,7 +4481,7 @@
         <v>18</v>
       </c>
       <c r="E162" s="1">
-        <v>1821.8</v>
+        <v>1942.5</v>
       </c>
       <c r="F162" s="1">
         <v>10</v>
@@ -4512,7 +4506,7 @@
         <v>17</v>
       </c>
       <c r="E163" s="1">
-        <v>2903.5</v>
+        <v>2668.5</v>
       </c>
       <c r="F163" s="1">
         <v>10</v>
@@ -4537,7 +4531,7 @@
         <v>12</v>
       </c>
       <c r="E164" s="1">
-        <v>659</v>
+        <v>639</v>
       </c>
       <c r="F164" s="1">
         <v>11</v>
@@ -4562,7 +4556,7 @@
         <v>18</v>
       </c>
       <c r="E165" s="1">
-        <v>1794.7</v>
+        <v>1915</v>
       </c>
       <c r="F165" s="1">
         <v>11</v>
@@ -4587,7 +4581,7 @@
         <v>17</v>
       </c>
       <c r="E166" s="1">
-        <v>2829.1</v>
+        <v>2593</v>
       </c>
       <c r="F166" s="1">
         <v>11</v>
@@ -4612,7 +4606,7 @@
         <v>12</v>
       </c>
       <c r="E167" s="1">
-        <v>653.29999999999995</v>
+        <v>637</v>
       </c>
       <c r="F167" s="1">
         <v>11</v>
@@ -4637,7 +4631,7 @@
         <v>18</v>
       </c>
       <c r="E168" s="1">
-        <v>1816.3</v>
+        <v>1967.5</v>
       </c>
       <c r="F168" s="1">
         <v>11</v>
@@ -4662,7 +4656,7 @@
         <v>17</v>
       </c>
       <c r="E169" s="1">
-        <v>2906.1</v>
+        <v>2648.5</v>
       </c>
       <c r="F169" s="1">
         <v>11</v>
@@ -4687,7 +4681,7 @@
         <v>12</v>
       </c>
       <c r="E170" s="1">
-        <v>652.79999999999995</v>
+        <v>656</v>
       </c>
       <c r="F170" s="1">
         <v>9</v>
@@ -4712,7 +4706,7 @@
         <v>18</v>
       </c>
       <c r="E171" s="1">
-        <v>1792</v>
+        <v>1941.5</v>
       </c>
       <c r="F171" s="1">
         <v>9</v>
@@ -4737,7 +4731,7 @@
         <v>17</v>
       </c>
       <c r="E172" s="1">
-        <v>2823.7</v>
+        <v>2642.5</v>
       </c>
       <c r="F172" s="1">
         <v>9</v>
@@ -4762,7 +4756,7 @@
         <v>12</v>
       </c>
       <c r="E173" s="1">
-        <v>682.7</v>
+        <v>675</v>
       </c>
       <c r="F173" s="1">
         <v>10</v>
@@ -4787,7 +4781,7 @@
         <v>18</v>
       </c>
       <c r="E174" s="1">
-        <v>1818</v>
+        <v>1983</v>
       </c>
       <c r="F174" s="1">
         <v>10</v>
@@ -4812,7 +4806,7 @@
         <v>17</v>
       </c>
       <c r="E175" s="1">
-        <v>2920.3</v>
+        <v>2681.5</v>
       </c>
       <c r="F175" s="1">
         <v>10</v>
@@ -4835,7 +4829,7 @@
         <v>12</v>
       </c>
       <c r="E176" s="1">
-        <v>628.29999999999995</v>
+        <v>627</v>
       </c>
       <c r="F176" s="1">
         <v>27</v>
@@ -4858,7 +4852,7 @@
         <v>18</v>
       </c>
       <c r="E177" s="1">
-        <v>1761.3</v>
+        <v>1918</v>
       </c>
       <c r="F177" s="1">
         <v>27</v>
@@ -4881,7 +4875,7 @@
         <v>17</v>
       </c>
       <c r="E178" s="1">
-        <v>2874.4</v>
+        <v>2587.5</v>
       </c>
       <c r="F178" s="1">
         <v>27</v>

</xml_diff>

<commit_message>
Added nominal formant frequency data for one study.
</commit_message>
<xml_diff>
--- a/inst/default_parameters.xlsx
+++ b/inst/default_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frkkan96/Documents/src/reindeer/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA92B03-62E0-2E47-B9C0-18EDEF54CA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D5D865-AF65-BF43-801C-EE718F3E5DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="500" windowWidth="25580" windowHeight="28300" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
+    <workbookView xWindow="37520" yWindow="1020" windowWidth="25580" windowHeight="28300" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="56">
   <si>
     <t>Gender</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>10.1044/2015_AJSLP-15-0020</t>
+  </si>
+  <si>
+    <t>10.1016/S0892-1997(99)80011-3</t>
   </si>
 </sst>
 </file>
@@ -628,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3287FC8-0847-0B47-A33C-7A45B3569376}">
-  <dimension ref="A1:G508"/>
+  <dimension ref="A1:G512"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A495" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
+      <selection activeCell="E522" sqref="E522"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12737,6 +12740,102 @@
       </c>
       <c r="G508" s="2" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="509" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A509" t="s">
+        <v>5</v>
+      </c>
+      <c r="B509">
+        <v>11</v>
+      </c>
+      <c r="C509">
+        <v>11</v>
+      </c>
+      <c r="D509" t="s">
+        <v>12</v>
+      </c>
+      <c r="E509" s="1">
+        <f>AVERAGE(387,967)</f>
+        <v>677</v>
+      </c>
+      <c r="F509" s="1">
+        <v>19</v>
+      </c>
+      <c r="G509" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="510" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A510" t="s">
+        <v>5</v>
+      </c>
+      <c r="B510">
+        <v>11</v>
+      </c>
+      <c r="C510">
+        <v>11</v>
+      </c>
+      <c r="D510" t="s">
+        <v>18</v>
+      </c>
+      <c r="E510" s="1">
+        <f>AVERAGE(2623,862)</f>
+        <v>1742.5</v>
+      </c>
+      <c r="F510" s="1">
+        <v>19</v>
+      </c>
+      <c r="G510" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="511" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A511" t="s">
+        <v>1</v>
+      </c>
+      <c r="B511">
+        <v>11</v>
+      </c>
+      <c r="C511">
+        <v>11</v>
+      </c>
+      <c r="D511" t="s">
+        <v>12</v>
+      </c>
+      <c r="E511" s="1">
+        <f>AVERAGE(912,362)</f>
+        <v>637</v>
+      </c>
+      <c r="F511" s="1">
+        <v>11</v>
+      </c>
+      <c r="G511" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="512" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A512" t="s">
+        <v>1</v>
+      </c>
+      <c r="B512">
+        <v>11</v>
+      </c>
+      <c r="C512">
+        <v>11</v>
+      </c>
+      <c r="D512" t="s">
+        <v>18</v>
+      </c>
+      <c r="E512" s="1">
+        <f>AVERAGE(2506,768)</f>
+        <v>1637</v>
+      </c>
+      <c r="F512" s="1">
+        <v>11</v>
+      </c>
+      <c r="G512" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -12787,9 +12886,11 @@
     <hyperlink ref="G21" r:id="rId44" display="https://doi.org/10.1044/2015_AJSLP-15-0020" xr:uid="{87B234FE-1A26-BD4A-947B-FB1F543777EB}"/>
     <hyperlink ref="G22" r:id="rId45" display="https://doi.org/10.1044/2015_AJSLP-15-0020" xr:uid="{09142B47-8E14-9742-B853-468362F70D85}"/>
     <hyperlink ref="G23:G24" r:id="rId46" display="https://doi.org/10.1044/2015_AJSLP-15-0020" xr:uid="{B24C93BF-6FB5-8A41-AF83-5523FD1896F5}"/>
+    <hyperlink ref="G509" r:id="rId47" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/S0892-1997(99)80011-3" xr:uid="{D7089C36-C646-C24E-8461-A834CF69C5DA}"/>
+    <hyperlink ref="G510:G512" r:id="rId48" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/S0892-1997(99)80011-3" xr:uid="{0AE3F141-6ABA-384C-8F34-4564C75A4524}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId47"/>
+  <legacyDrawing r:id="rId49"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added pitch range data for smaller children
</commit_message>
<xml_diff>
--- a/inst/default_parameters.xlsx
+++ b/inst/default_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frkkan96/Documents/src/reindeer/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D5D865-AF65-BF43-801C-EE718F3E5DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CBFEEE-1D3B-C547-A07C-53B75FE2A2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37520" yWindow="1020" windowWidth="25580" windowHeight="28300" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
+    <workbookView xWindow="25620" yWindow="500" windowWidth="25580" windowHeight="28300" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="57">
   <si>
     <t>Gender</t>
   </si>
@@ -230,14 +230,18 @@
   <si>
     <t>10.1016/S0892-1997(99)80011-3</t>
   </si>
+  <si>
+    <t>10.1016/j.ijporl.2008.12.005</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -292,12 +296,14 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlänk" xfId="2" builtinId="8"/>
@@ -631,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3287FC8-0847-0B47-A33C-7A45B3569376}">
-  <dimension ref="A1:G512"/>
+  <dimension ref="A1:G596"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A495" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
-      <selection activeCell="E522" sqref="E522"/>
+    <sheetView tabSelected="1" topLeftCell="A521" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
+      <selection activeCell="G537" sqref="G537:G596"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12836,6 +12842,1942 @@
       </c>
       <c r="G512" s="2" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="513" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A513" t="s">
+        <v>1</v>
+      </c>
+      <c r="B513">
+        <v>2</v>
+      </c>
+      <c r="C513">
+        <v>2</v>
+      </c>
+      <c r="D513" t="s">
+        <v>10</v>
+      </c>
+      <c r="E513" s="1">
+        <v>268</v>
+      </c>
+      <c r="F513" s="1">
+        <v>3</v>
+      </c>
+      <c r="G513" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="514" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A514" t="s">
+        <v>1</v>
+      </c>
+      <c r="B514">
+        <v>2</v>
+      </c>
+      <c r="C514">
+        <v>2</v>
+      </c>
+      <c r="D514" t="s">
+        <v>9</v>
+      </c>
+      <c r="E514" s="1">
+        <v>378</v>
+      </c>
+      <c r="F514" s="1">
+        <v>3</v>
+      </c>
+      <c r="G514" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="515" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A515" t="s">
+        <v>5</v>
+      </c>
+      <c r="B515">
+        <v>2</v>
+      </c>
+      <c r="C515">
+        <v>2</v>
+      </c>
+      <c r="D515" t="s">
+        <v>10</v>
+      </c>
+      <c r="E515" s="1">
+        <v>268</v>
+      </c>
+      <c r="F515" s="1">
+        <v>3</v>
+      </c>
+      <c r="G515" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="516" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A516" t="s">
+        <v>5</v>
+      </c>
+      <c r="B516">
+        <v>2</v>
+      </c>
+      <c r="C516">
+        <v>2</v>
+      </c>
+      <c r="D516" t="s">
+        <v>9</v>
+      </c>
+      <c r="E516" s="1">
+        <v>378</v>
+      </c>
+      <c r="F516" s="1">
+        <v>3</v>
+      </c>
+      <c r="G516" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="517" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A517" t="s">
+        <v>1</v>
+      </c>
+      <c r="B517">
+        <v>2</v>
+      </c>
+      <c r="C517">
+        <v>2.16</v>
+      </c>
+      <c r="D517" t="s">
+        <v>10</v>
+      </c>
+      <c r="E517" s="1">
+        <v>297</v>
+      </c>
+      <c r="F517" s="1">
+        <v>3</v>
+      </c>
+      <c r="G517" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="518" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A518" t="s">
+        <v>1</v>
+      </c>
+      <c r="B518">
+        <v>2</v>
+      </c>
+      <c r="C518">
+        <v>2.16</v>
+      </c>
+      <c r="D518" t="s">
+        <v>9</v>
+      </c>
+      <c r="E518" s="1">
+        <v>453</v>
+      </c>
+      <c r="F518" s="1">
+        <v>3</v>
+      </c>
+      <c r="G518" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="519" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A519" t="s">
+        <v>5</v>
+      </c>
+      <c r="B519">
+        <v>2</v>
+      </c>
+      <c r="C519">
+        <v>2.16</v>
+      </c>
+      <c r="D519" t="s">
+        <v>10</v>
+      </c>
+      <c r="E519" s="1">
+        <v>297</v>
+      </c>
+      <c r="F519" s="1">
+        <v>3</v>
+      </c>
+      <c r="G519" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="520" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A520" t="s">
+        <v>5</v>
+      </c>
+      <c r="B520">
+        <v>2</v>
+      </c>
+      <c r="C520">
+        <v>2.16</v>
+      </c>
+      <c r="D520" t="s">
+        <v>9</v>
+      </c>
+      <c r="E520" s="1">
+        <v>453</v>
+      </c>
+      <c r="F520" s="1">
+        <v>3</v>
+      </c>
+      <c r="G520" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="521" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A521" t="s">
+        <v>1</v>
+      </c>
+      <c r="B521">
+        <v>4</v>
+      </c>
+      <c r="C521">
+        <v>4</v>
+      </c>
+      <c r="D521" t="s">
+        <v>10</v>
+      </c>
+      <c r="E521" s="1">
+        <v>270</v>
+      </c>
+      <c r="F521" s="1">
+        <v>4</v>
+      </c>
+      <c r="G521" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="522" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A522" t="s">
+        <v>1</v>
+      </c>
+      <c r="B522">
+        <v>4</v>
+      </c>
+      <c r="C522">
+        <v>4</v>
+      </c>
+      <c r="D522" t="s">
+        <v>9</v>
+      </c>
+      <c r="E522" s="1">
+        <v>560</v>
+      </c>
+      <c r="F522" s="1">
+        <v>4</v>
+      </c>
+      <c r="G522" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="523" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A523" t="s">
+        <v>5</v>
+      </c>
+      <c r="B523">
+        <v>4</v>
+      </c>
+      <c r="C523">
+        <v>4</v>
+      </c>
+      <c r="D523" t="s">
+        <v>10</v>
+      </c>
+      <c r="E523" s="1">
+        <v>270</v>
+      </c>
+      <c r="F523" s="1">
+        <v>4</v>
+      </c>
+      <c r="G523" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="524" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A524" t="s">
+        <v>5</v>
+      </c>
+      <c r="B524">
+        <v>4</v>
+      </c>
+      <c r="C524">
+        <v>4</v>
+      </c>
+      <c r="D524" t="s">
+        <v>9</v>
+      </c>
+      <c r="E524" s="1">
+        <v>560</v>
+      </c>
+      <c r="F524" s="1">
+        <v>4</v>
+      </c>
+      <c r="G524" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="525" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A525" t="s">
+        <v>1</v>
+      </c>
+      <c r="B525">
+        <v>3</v>
+      </c>
+      <c r="C525">
+        <v>3</v>
+      </c>
+      <c r="D525" t="s">
+        <v>10</v>
+      </c>
+      <c r="E525" s="1">
+        <v>209</v>
+      </c>
+      <c r="F525" s="1">
+        <v>10</v>
+      </c>
+      <c r="G525" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="526" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A526" t="s">
+        <v>1</v>
+      </c>
+      <c r="B526">
+        <v>3</v>
+      </c>
+      <c r="C526">
+        <v>3</v>
+      </c>
+      <c r="D526" t="s">
+        <v>9</v>
+      </c>
+      <c r="E526" s="1">
+        <v>271</v>
+      </c>
+      <c r="F526" s="1">
+        <v>10</v>
+      </c>
+      <c r="G526" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="527" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A527" t="s">
+        <v>5</v>
+      </c>
+      <c r="B527">
+        <v>3</v>
+      </c>
+      <c r="C527">
+        <v>3</v>
+      </c>
+      <c r="D527" t="s">
+        <v>10</v>
+      </c>
+      <c r="E527" s="1">
+        <v>209</v>
+      </c>
+      <c r="F527" s="1">
+        <v>10</v>
+      </c>
+      <c r="G527" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="528" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A528" t="s">
+        <v>5</v>
+      </c>
+      <c r="B528">
+        <v>3</v>
+      </c>
+      <c r="C528">
+        <v>3</v>
+      </c>
+      <c r="D528" t="s">
+        <v>9</v>
+      </c>
+      <c r="E528" s="1">
+        <v>271</v>
+      </c>
+      <c r="F528" s="1">
+        <v>10</v>
+      </c>
+      <c r="G528" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="529" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A529" t="s">
+        <v>1</v>
+      </c>
+      <c r="B529">
+        <v>4.5</v>
+      </c>
+      <c r="C529">
+        <v>4.5</v>
+      </c>
+      <c r="D529" t="s">
+        <v>10</v>
+      </c>
+      <c r="E529" s="1">
+        <v>276</v>
+      </c>
+      <c r="F529" s="1">
+        <v>10</v>
+      </c>
+      <c r="G529" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="530" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A530" t="s">
+        <v>1</v>
+      </c>
+      <c r="B530">
+        <v>4.5</v>
+      </c>
+      <c r="C530">
+        <v>4.5</v>
+      </c>
+      <c r="D530" t="s">
+        <v>9</v>
+      </c>
+      <c r="E530" s="1">
+        <v>323</v>
+      </c>
+      <c r="F530" s="1">
+        <v>10</v>
+      </c>
+      <c r="G530" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="531" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A531" t="s">
+        <v>5</v>
+      </c>
+      <c r="B531">
+        <v>4.5</v>
+      </c>
+      <c r="C531">
+        <v>4.5</v>
+      </c>
+      <c r="D531" t="s">
+        <v>10</v>
+      </c>
+      <c r="E531" s="1">
+        <v>276</v>
+      </c>
+      <c r="F531" s="1">
+        <v>10</v>
+      </c>
+      <c r="G531" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="532" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A532" t="s">
+        <v>5</v>
+      </c>
+      <c r="B532">
+        <v>4.5</v>
+      </c>
+      <c r="C532">
+        <v>4.5</v>
+      </c>
+      <c r="D532" t="s">
+        <v>9</v>
+      </c>
+      <c r="E532" s="1">
+        <v>323</v>
+      </c>
+      <c r="F532" s="1">
+        <v>10</v>
+      </c>
+      <c r="G532" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="533" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A533" t="s">
+        <v>1</v>
+      </c>
+      <c r="B533">
+        <v>4.25</v>
+      </c>
+      <c r="C533">
+        <v>4.25</v>
+      </c>
+      <c r="D533" t="s">
+        <v>10</v>
+      </c>
+      <c r="E533" s="1">
+        <v>217</v>
+      </c>
+      <c r="F533" s="1">
+        <v>15</v>
+      </c>
+      <c r="G533" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="534" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A534" t="s">
+        <v>1</v>
+      </c>
+      <c r="B534">
+        <v>4.25</v>
+      </c>
+      <c r="C534">
+        <v>4.25</v>
+      </c>
+      <c r="D534" t="s">
+        <v>9</v>
+      </c>
+      <c r="E534" s="1">
+        <v>295</v>
+      </c>
+      <c r="F534" s="1">
+        <v>15</v>
+      </c>
+      <c r="G534" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="535" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A535" t="s">
+        <v>5</v>
+      </c>
+      <c r="B535">
+        <v>4.25</v>
+      </c>
+      <c r="C535">
+        <v>4.25</v>
+      </c>
+      <c r="D535" t="s">
+        <v>10</v>
+      </c>
+      <c r="E535" s="1">
+        <v>217</v>
+      </c>
+      <c r="F535" s="1">
+        <v>18</v>
+      </c>
+      <c r="G535" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="536" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A536" t="s">
+        <v>5</v>
+      </c>
+      <c r="B536">
+        <v>4.25</v>
+      </c>
+      <c r="C536">
+        <v>4.25</v>
+      </c>
+      <c r="D536" t="s">
+        <v>9</v>
+      </c>
+      <c r="E536" s="1">
+        <v>295</v>
+      </c>
+      <c r="F536" s="1">
+        <v>18</v>
+      </c>
+      <c r="G536" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="537" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A537" t="s">
+        <v>1</v>
+      </c>
+      <c r="B537">
+        <v>5</v>
+      </c>
+      <c r="C537">
+        <v>5</v>
+      </c>
+      <c r="D537" t="s">
+        <v>10</v>
+      </c>
+      <c r="E537" s="1">
+        <v>240</v>
+      </c>
+      <c r="F537" s="1">
+        <v>5</v>
+      </c>
+      <c r="G537" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="538" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A538" t="s">
+        <v>1</v>
+      </c>
+      <c r="B538">
+        <v>5</v>
+      </c>
+      <c r="C538">
+        <v>5</v>
+      </c>
+      <c r="D538" t="s">
+        <v>9</v>
+      </c>
+      <c r="E538" s="1">
+        <v>280</v>
+      </c>
+      <c r="F538" s="1">
+        <v>5</v>
+      </c>
+      <c r="G538" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="539" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A539" t="s">
+        <v>5</v>
+      </c>
+      <c r="B539">
+        <v>5</v>
+      </c>
+      <c r="C539">
+        <v>5</v>
+      </c>
+      <c r="D539" t="s">
+        <v>10</v>
+      </c>
+      <c r="E539" s="1">
+        <v>240</v>
+      </c>
+      <c r="F539" s="1">
+        <v>5</v>
+      </c>
+      <c r="G539" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="540" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A540" t="s">
+        <v>5</v>
+      </c>
+      <c r="B540">
+        <v>5</v>
+      </c>
+      <c r="C540">
+        <v>5</v>
+      </c>
+      <c r="D540" t="s">
+        <v>9</v>
+      </c>
+      <c r="E540" s="1">
+        <v>280</v>
+      </c>
+      <c r="F540" s="1">
+        <v>5</v>
+      </c>
+      <c r="G540" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="541" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A541" t="s">
+        <v>1</v>
+      </c>
+      <c r="B541">
+        <v>5</v>
+      </c>
+      <c r="C541">
+        <v>5</v>
+      </c>
+      <c r="D541" t="s">
+        <v>10</v>
+      </c>
+      <c r="E541" s="1">
+        <v>186</v>
+      </c>
+      <c r="F541" s="1">
+        <v>15</v>
+      </c>
+      <c r="G541" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="542" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A542" t="s">
+        <v>1</v>
+      </c>
+      <c r="B542">
+        <v>5</v>
+      </c>
+      <c r="C542">
+        <v>5</v>
+      </c>
+      <c r="D542" t="s">
+        <v>9</v>
+      </c>
+      <c r="E542" s="1">
+        <v>313</v>
+      </c>
+      <c r="F542" s="1">
+        <v>15</v>
+      </c>
+      <c r="G542" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="543" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A543" t="s">
+        <v>5</v>
+      </c>
+      <c r="B543">
+        <v>5</v>
+      </c>
+      <c r="C543">
+        <v>5</v>
+      </c>
+      <c r="D543" t="s">
+        <v>10</v>
+      </c>
+      <c r="E543" s="1">
+        <v>202</v>
+      </c>
+      <c r="F543" s="1">
+        <v>15</v>
+      </c>
+      <c r="G543" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="544" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A544" t="s">
+        <v>5</v>
+      </c>
+      <c r="B544">
+        <v>5</v>
+      </c>
+      <c r="C544">
+        <v>5</v>
+      </c>
+      <c r="D544" t="s">
+        <v>9</v>
+      </c>
+      <c r="E544" s="1">
+        <v>306</v>
+      </c>
+      <c r="F544" s="1">
+        <v>15</v>
+      </c>
+      <c r="G544" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="545" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A545" t="s">
+        <v>1</v>
+      </c>
+      <c r="B545">
+        <v>5.6</v>
+      </c>
+      <c r="C545">
+        <v>5.6</v>
+      </c>
+      <c r="D545" t="s">
+        <v>10</v>
+      </c>
+      <c r="E545" s="1">
+        <v>260</v>
+      </c>
+      <c r="F545" s="1">
+        <v>19</v>
+      </c>
+      <c r="G545" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="546" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A546" t="s">
+        <v>1</v>
+      </c>
+      <c r="B546">
+        <v>5.6</v>
+      </c>
+      <c r="C546">
+        <v>5.6</v>
+      </c>
+      <c r="D546" t="s">
+        <v>9</v>
+      </c>
+      <c r="E546" s="1">
+        <v>287</v>
+      </c>
+      <c r="F546" s="1">
+        <v>19</v>
+      </c>
+      <c r="G546" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="547" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A547" t="s">
+        <v>5</v>
+      </c>
+      <c r="B547">
+        <v>5.5</v>
+      </c>
+      <c r="C547">
+        <v>5.5</v>
+      </c>
+      <c r="D547" t="s">
+        <v>10</v>
+      </c>
+      <c r="E547" s="1">
+        <v>258</v>
+      </c>
+      <c r="F547" s="1">
+        <v>13</v>
+      </c>
+      <c r="G547" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="548" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A548" t="s">
+        <v>5</v>
+      </c>
+      <c r="B548">
+        <v>5.5</v>
+      </c>
+      <c r="C548">
+        <v>5.5</v>
+      </c>
+      <c r="D548" t="s">
+        <v>9</v>
+      </c>
+      <c r="E548" s="1">
+        <v>300</v>
+      </c>
+      <c r="F548" s="1">
+        <v>13</v>
+      </c>
+      <c r="G548" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="549" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A549" t="s">
+        <v>1</v>
+      </c>
+      <c r="B549">
+        <v>5.5</v>
+      </c>
+      <c r="C549">
+        <v>5.5</v>
+      </c>
+      <c r="D549" t="s">
+        <v>10</v>
+      </c>
+      <c r="E549" s="1">
+        <v>217</v>
+      </c>
+      <c r="F549" s="1">
+        <v>15</v>
+      </c>
+      <c r="G549" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="550" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A550" t="s">
+        <v>1</v>
+      </c>
+      <c r="B550">
+        <v>5.5</v>
+      </c>
+      <c r="C550">
+        <v>5.5</v>
+      </c>
+      <c r="D550" t="s">
+        <v>9</v>
+      </c>
+      <c r="E550" s="1">
+        <v>293</v>
+      </c>
+      <c r="F550" s="1">
+        <v>15</v>
+      </c>
+      <c r="G550" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="551" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A551" t="s">
+        <v>5</v>
+      </c>
+      <c r="B551">
+        <v>5.5</v>
+      </c>
+      <c r="C551">
+        <v>5.5</v>
+      </c>
+      <c r="D551" t="s">
+        <v>10</v>
+      </c>
+      <c r="E551" s="1">
+        <v>212</v>
+      </c>
+      <c r="F551" s="1">
+        <v>18</v>
+      </c>
+      <c r="G551" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="552" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A552" t="s">
+        <v>5</v>
+      </c>
+      <c r="B552">
+        <v>5.5</v>
+      </c>
+      <c r="C552">
+        <v>5.5</v>
+      </c>
+      <c r="D552" t="s">
+        <v>9</v>
+      </c>
+      <c r="E552" s="1">
+        <v>295</v>
+      </c>
+      <c r="F552" s="1">
+        <v>16</v>
+      </c>
+      <c r="G552" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="553" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A553" t="s">
+        <v>1</v>
+      </c>
+      <c r="B553">
+        <v>5.5</v>
+      </c>
+      <c r="C553">
+        <v>5.5</v>
+      </c>
+      <c r="D553" t="s">
+        <v>10</v>
+      </c>
+      <c r="E553" s="1">
+        <v>205</v>
+      </c>
+      <c r="F553" s="1">
+        <v>18</v>
+      </c>
+      <c r="G553" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="554" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A554" t="s">
+        <v>1</v>
+      </c>
+      <c r="B554">
+        <v>5.5</v>
+      </c>
+      <c r="C554">
+        <v>5.5</v>
+      </c>
+      <c r="D554" t="s">
+        <v>9</v>
+      </c>
+      <c r="E554" s="1">
+        <v>274</v>
+      </c>
+      <c r="F554" s="1">
+        <v>18</v>
+      </c>
+      <c r="G554" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="555" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A555" t="s">
+        <v>5</v>
+      </c>
+      <c r="B555">
+        <v>5.5</v>
+      </c>
+      <c r="C555">
+        <v>5.5</v>
+      </c>
+      <c r="D555" t="s">
+        <v>10</v>
+      </c>
+      <c r="E555" s="1">
+        <v>208</v>
+      </c>
+      <c r="F555" s="1">
+        <v>17</v>
+      </c>
+      <c r="G555" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="556" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A556" t="s">
+        <v>5</v>
+      </c>
+      <c r="B556">
+        <v>5.5</v>
+      </c>
+      <c r="C556">
+        <v>5.5</v>
+      </c>
+      <c r="D556" t="s">
+        <v>9</v>
+      </c>
+      <c r="E556" s="1">
+        <v>262</v>
+      </c>
+      <c r="F556" s="1">
+        <v>17</v>
+      </c>
+      <c r="G556" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="557" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A557" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B557" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="C557" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="D557" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E557" s="1">
+        <v>212</v>
+      </c>
+      <c r="F557" s="1">
+        <v>15</v>
+      </c>
+      <c r="G557" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="558" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A558" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B558" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="C558" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="D558" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E558" s="1">
+        <v>260</v>
+      </c>
+      <c r="F558" s="1">
+        <v>15</v>
+      </c>
+      <c r="G558" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="559" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A559" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B559" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="C559" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="D559" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E559" s="1">
+        <v>195</v>
+      </c>
+      <c r="F559" s="1">
+        <v>20</v>
+      </c>
+      <c r="G559" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="560" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A560" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B560" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="C560" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="D560" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E560" s="1">
+        <v>291</v>
+      </c>
+      <c r="F560" s="1">
+        <v>20</v>
+      </c>
+      <c r="G560" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="561" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A561" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B561" s="3">
+        <v>6</v>
+      </c>
+      <c r="C561" s="3">
+        <v>6</v>
+      </c>
+      <c r="D561" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E561" s="1">
+        <v>212</v>
+      </c>
+      <c r="F561" s="1">
+        <v>7</v>
+      </c>
+      <c r="G561" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="562" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A562" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B562" s="3">
+        <v>6</v>
+      </c>
+      <c r="C562" s="3">
+        <v>6</v>
+      </c>
+      <c r="D562" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E562" s="1">
+        <v>280</v>
+      </c>
+      <c r="F562" s="1">
+        <v>7</v>
+      </c>
+      <c r="G562" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="563" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A563" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B563" s="3">
+        <v>6</v>
+      </c>
+      <c r="C563" s="3">
+        <v>6</v>
+      </c>
+      <c r="D563" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E563" s="1">
+        <v>212</v>
+      </c>
+      <c r="F563" s="1">
+        <v>8</v>
+      </c>
+      <c r="G563" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="564" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A564" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B564" s="3">
+        <v>6</v>
+      </c>
+      <c r="C564" s="3">
+        <v>6</v>
+      </c>
+      <c r="D564" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E564" s="1">
+        <v>280</v>
+      </c>
+      <c r="F564" s="1">
+        <v>8</v>
+      </c>
+      <c r="G564" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="565" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A565" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B565" s="3">
+        <v>6</v>
+      </c>
+      <c r="C565" s="3">
+        <v>6</v>
+      </c>
+      <c r="D565" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E565" s="1">
+        <v>204</v>
+      </c>
+      <c r="F565" s="1">
+        <v>14</v>
+      </c>
+      <c r="G565" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="566" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A566" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B566" s="3">
+        <v>6</v>
+      </c>
+      <c r="C566" s="3">
+        <v>6</v>
+      </c>
+      <c r="D566" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E566" s="1">
+        <v>274</v>
+      </c>
+      <c r="F566" s="1">
+        <v>14</v>
+      </c>
+      <c r="G566" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="567" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A567" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B567" s="3">
+        <v>6</v>
+      </c>
+      <c r="C567" s="3">
+        <v>6</v>
+      </c>
+      <c r="D567" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E567" s="1">
+        <v>218</v>
+      </c>
+      <c r="F567" s="1">
+        <v>19</v>
+      </c>
+      <c r="G567" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="568" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A568" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B568" s="3">
+        <v>6</v>
+      </c>
+      <c r="C568" s="3">
+        <v>6</v>
+      </c>
+      <c r="D568" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E568" s="1">
+        <v>274</v>
+      </c>
+      <c r="F568" s="1">
+        <v>19</v>
+      </c>
+      <c r="G568" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="569" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A569" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B569" s="3">
+        <v>6</v>
+      </c>
+      <c r="C569" s="3">
+        <v>6</v>
+      </c>
+      <c r="D569" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E569" s="1">
+        <v>228</v>
+      </c>
+      <c r="F569" s="1">
+        <v>15</v>
+      </c>
+      <c r="G569" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="570" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A570" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B570" s="3">
+        <v>6</v>
+      </c>
+      <c r="C570" s="3">
+        <v>6</v>
+      </c>
+      <c r="D570" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E570" s="1">
+        <v>332</v>
+      </c>
+      <c r="F570" s="1">
+        <v>15</v>
+      </c>
+      <c r="G570" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="571" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A571" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B571" s="3">
+        <v>6</v>
+      </c>
+      <c r="C571" s="3">
+        <v>6</v>
+      </c>
+      <c r="D571" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E571" s="1">
+        <v>210</v>
+      </c>
+      <c r="F571" s="1">
+        <v>15</v>
+      </c>
+      <c r="G571" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="572" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A572" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B572" s="3">
+        <v>6</v>
+      </c>
+      <c r="C572" s="3">
+        <v>6</v>
+      </c>
+      <c r="D572" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E572" s="1">
+        <v>313</v>
+      </c>
+      <c r="F572" s="1">
+        <v>15</v>
+      </c>
+      <c r="G572" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="573" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A573" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B573" s="3">
+        <v>6</v>
+      </c>
+      <c r="C573" s="3">
+        <v>6</v>
+      </c>
+      <c r="D573" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E573" s="1">
+        <v>135</v>
+      </c>
+      <c r="F573" s="1">
+        <v>50</v>
+      </c>
+      <c r="G573" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="574" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A574" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B574" s="3">
+        <v>6</v>
+      </c>
+      <c r="C574" s="3">
+        <v>6</v>
+      </c>
+      <c r="D574" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E574" s="1">
+        <v>299</v>
+      </c>
+      <c r="F574" s="1">
+        <v>50</v>
+      </c>
+      <c r="G574" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="575" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A575" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B575" s="3">
+        <v>6</v>
+      </c>
+      <c r="C575" s="3">
+        <v>6</v>
+      </c>
+      <c r="D575" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E575" s="1">
+        <v>138</v>
+      </c>
+      <c r="F575" s="1">
+        <v>50</v>
+      </c>
+      <c r="G575" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="576" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A576" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B576" s="3">
+        <v>6</v>
+      </c>
+      <c r="C576" s="3">
+        <v>6</v>
+      </c>
+      <c r="D576" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E576" s="1">
+        <v>298</v>
+      </c>
+      <c r="F576" s="1">
+        <v>50</v>
+      </c>
+      <c r="G576" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="577" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A577" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B577" s="3">
+        <v>6</v>
+      </c>
+      <c r="C577" s="3">
+        <v>6</v>
+      </c>
+      <c r="D577" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E577" s="1">
+        <v>253</v>
+      </c>
+      <c r="F577" s="1">
+        <v>3</v>
+      </c>
+      <c r="G577" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="578" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A578" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B578" s="3">
+        <v>6</v>
+      </c>
+      <c r="C578" s="3">
+        <v>6</v>
+      </c>
+      <c r="D578" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E578" s="1">
+        <v>185</v>
+      </c>
+      <c r="F578" s="1">
+        <v>3</v>
+      </c>
+      <c r="G578" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="579" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A579" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B579" s="3">
+        <v>6</v>
+      </c>
+      <c r="C579" s="3">
+        <v>6</v>
+      </c>
+      <c r="D579" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E579" s="1">
+        <v>194</v>
+      </c>
+      <c r="F579" s="1">
+        <v>3</v>
+      </c>
+      <c r="G579" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="580" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A580" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B580" s="3">
+        <v>6</v>
+      </c>
+      <c r="C580" s="3">
+        <v>6</v>
+      </c>
+      <c r="D580" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E580" s="1">
+        <v>325</v>
+      </c>
+      <c r="F580" s="1">
+        <v>3</v>
+      </c>
+      <c r="G580" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="581" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A581" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B581" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="C581" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="D581" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E581" s="1">
+        <v>204</v>
+      </c>
+      <c r="F581" s="1">
+        <v>14</v>
+      </c>
+      <c r="G581" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="582" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A582" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B582" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="C582" s="5">
+        <v>6.5</v>
+      </c>
+      <c r="D582" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E582" s="1">
+        <v>274</v>
+      </c>
+      <c r="F582" s="1">
+        <v>14</v>
+      </c>
+      <c r="G582" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="583" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A583" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B583" s="5">
+        <f>6+4/12</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="C583" s="5">
+        <f t="shared" ref="C583:C584" si="15">6+4/12</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="D583" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E583" s="1">
+        <v>218</v>
+      </c>
+      <c r="F583" s="1">
+        <v>19</v>
+      </c>
+      <c r="G583" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="584" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A584" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B584" s="5">
+        <f t="shared" ref="B584:C584" si="16">6+4/12</f>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="C584" s="5">
+        <f t="shared" si="15"/>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="D584" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E584" s="1">
+        <v>274</v>
+      </c>
+      <c r="F584" s="1">
+        <v>19</v>
+      </c>
+      <c r="G584" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="585" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A585" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B585" s="6">
+        <v>7</v>
+      </c>
+      <c r="C585" s="6">
+        <v>7</v>
+      </c>
+      <c r="D585" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E585" s="1">
+        <v>208</v>
+      </c>
+      <c r="F585" s="1">
+        <v>5</v>
+      </c>
+      <c r="G585" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="586" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A586" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B586" s="6">
+        <v>7</v>
+      </c>
+      <c r="C586" s="6">
+        <v>7</v>
+      </c>
+      <c r="D586" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E586" s="1">
+        <v>257</v>
+      </c>
+      <c r="F586" s="1">
+        <v>5</v>
+      </c>
+      <c r="G586" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="587" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A587" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B587" s="6">
+        <v>7</v>
+      </c>
+      <c r="C587" s="6">
+        <v>7</v>
+      </c>
+      <c r="D587" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E587" s="1">
+        <v>208</v>
+      </c>
+      <c r="F587" s="1">
+        <v>5</v>
+      </c>
+      <c r="G587" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="588" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A588" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B588" s="6">
+        <v>7</v>
+      </c>
+      <c r="C588" s="6">
+        <v>7</v>
+      </c>
+      <c r="D588" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E588" s="1">
+        <v>257</v>
+      </c>
+      <c r="F588" s="1">
+        <v>5</v>
+      </c>
+      <c r="G588" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="589" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A589" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B589" s="6">
+        <v>7</v>
+      </c>
+      <c r="C589" s="6">
+        <v>7</v>
+      </c>
+      <c r="D589" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E589" s="1">
+        <v>199</v>
+      </c>
+      <c r="F589" s="1">
+        <v>15</v>
+      </c>
+      <c r="G589" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="590" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A590" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B590" s="6">
+        <v>7</v>
+      </c>
+      <c r="C590" s="6">
+        <v>7</v>
+      </c>
+      <c r="D590" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E590" s="1">
+        <v>264</v>
+      </c>
+      <c r="F590" s="1">
+        <v>15</v>
+      </c>
+      <c r="G590" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="591" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A591" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B591" s="6">
+        <v>7</v>
+      </c>
+      <c r="C591" s="6">
+        <v>7</v>
+      </c>
+      <c r="D591" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E591" s="1">
+        <v>195</v>
+      </c>
+      <c r="F591" s="1">
+        <v>15</v>
+      </c>
+      <c r="G591" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="592" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A592" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B592" s="6">
+        <v>7</v>
+      </c>
+      <c r="C592" s="6">
+        <v>7</v>
+      </c>
+      <c r="D592" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E592" s="1">
+        <v>303</v>
+      </c>
+      <c r="F592" s="1">
+        <v>15</v>
+      </c>
+      <c r="G592" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="593" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A593" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B593" s="6">
+        <v>7</v>
+      </c>
+      <c r="C593" s="6">
+        <v>7</v>
+      </c>
+      <c r="D593" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E593" s="1">
+        <v>253</v>
+      </c>
+      <c r="F593" s="1">
+        <v>11</v>
+      </c>
+      <c r="G593" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="594" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A594" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B594" s="6">
+        <v>7</v>
+      </c>
+      <c r="C594" s="6">
+        <v>7</v>
+      </c>
+      <c r="D594" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E594" s="1">
+        <v>281</v>
+      </c>
+      <c r="F594" s="1">
+        <v>11</v>
+      </c>
+      <c r="G594" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="595" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A595" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B595" s="6">
+        <v>7</v>
+      </c>
+      <c r="C595" s="6">
+        <v>7</v>
+      </c>
+      <c r="D595" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E595" s="1">
+        <v>265</v>
+      </c>
+      <c r="F595" s="1">
+        <v>24</v>
+      </c>
+      <c r="G595" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="596" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A596" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B596" s="6">
+        <v>7</v>
+      </c>
+      <c r="C596" s="6">
+        <v>7</v>
+      </c>
+      <c r="D596" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E596" s="1">
+        <v>298</v>
+      </c>
+      <c r="F596" s="1">
+        <v>24</v>
+      </c>
+      <c r="G596" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Formant data from the Praat data sets.
</commit_message>
<xml_diff>
--- a/inst/default_parameters.xlsx
+++ b/inst/default_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frkkan96/Documents/src/reindeer/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CBFEEE-1D3B-C547-A07C-53B75FE2A2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FEC622-9800-5540-B7B1-3420106DE4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25620" yWindow="500" windowWidth="25580" windowHeight="28300" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1837" uniqueCount="60">
   <si>
     <t>Gender</t>
   </si>
@@ -233,6 +233,15 @@
   <si>
     <t>10.1016/j.ijporl.2008.12.005</t>
   </si>
+  <si>
+    <t>10.1121/1.1913429</t>
+  </si>
+  <si>
+    <t>10.1016/j.jcomdis.2015.10.007</t>
+  </si>
+  <si>
+    <t>10.1016/s0095-4470(19)31416-0 </t>
+  </si>
 </sst>
 </file>
 
@@ -241,7 +250,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -302,7 +311,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -637,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3287FC8-0847-0B47-A33C-7A45B3569376}">
-  <dimension ref="A1:G596"/>
+  <dimension ref="A1:G610"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A521" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
-      <selection activeCell="G537" sqref="G537:G596"/>
+    <sheetView tabSelected="1" topLeftCell="A580" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
+      <selection activeCell="B589" sqref="B589"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14484,7 +14493,7 @@
         <v>5</v>
       </c>
       <c r="B584" s="5">
-        <f t="shared" ref="B584:C584" si="16">6+4/12</f>
+        <f t="shared" ref="B584" si="16">6+4/12</f>
         <v>6.333333333333333</v>
       </c>
       <c r="C584" s="5">
@@ -14778,6 +14787,334 @@
       </c>
       <c r="G596" s="2" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="597" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A597" t="s">
+        <v>1</v>
+      </c>
+      <c r="B597">
+        <v>18</v>
+      </c>
+      <c r="C597">
+        <v>30</v>
+      </c>
+      <c r="D597" t="s">
+        <v>12</v>
+      </c>
+      <c r="E597" s="1">
+        <v>286</v>
+      </c>
+      <c r="F597" s="1">
+        <v>50</v>
+      </c>
+      <c r="G597" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="598" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A598" t="s">
+        <v>1</v>
+      </c>
+      <c r="B598">
+        <v>18</v>
+      </c>
+      <c r="C598">
+        <v>30</v>
+      </c>
+      <c r="D598" t="s">
+        <v>18</v>
+      </c>
+      <c r="E598" s="1">
+        <v>792</v>
+      </c>
+      <c r="F598" s="1">
+        <v>50</v>
+      </c>
+      <c r="G598" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="599" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A599" t="s">
+        <v>1</v>
+      </c>
+      <c r="B599">
+        <v>18</v>
+      </c>
+      <c r="C599">
+        <v>30</v>
+      </c>
+      <c r="D599" t="s">
+        <v>17</v>
+      </c>
+      <c r="E599" s="1">
+        <v>2128</v>
+      </c>
+      <c r="F599" s="1">
+        <v>50</v>
+      </c>
+      <c r="G599" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="600" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A600" t="s">
+        <v>5</v>
+      </c>
+      <c r="B600">
+        <v>18</v>
+      </c>
+      <c r="C600">
+        <v>30</v>
+      </c>
+      <c r="D600" t="s">
+        <v>12</v>
+      </c>
+      <c r="E600" s="1">
+        <v>270</v>
+      </c>
+      <c r="F600" s="1">
+        <v>25</v>
+      </c>
+      <c r="G600" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="601" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A601" t="s">
+        <v>5</v>
+      </c>
+      <c r="B601">
+        <v>18</v>
+      </c>
+      <c r="C601">
+        <v>30</v>
+      </c>
+      <c r="D601" t="s">
+        <v>18</v>
+      </c>
+      <c r="E601" s="1">
+        <v>807</v>
+      </c>
+      <c r="F601" s="1">
+        <v>25</v>
+      </c>
+      <c r="G601" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="602" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A602" t="s">
+        <v>5</v>
+      </c>
+      <c r="B602">
+        <v>18</v>
+      </c>
+      <c r="C602">
+        <v>30</v>
+      </c>
+      <c r="D602" t="s">
+        <v>17</v>
+      </c>
+      <c r="E602" s="1">
+        <v>2364</v>
+      </c>
+      <c r="F602" s="1">
+        <v>25</v>
+      </c>
+      <c r="G602" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="603" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A603" t="s">
+        <v>7</v>
+      </c>
+      <c r="B603">
+        <v>5</v>
+      </c>
+      <c r="C603">
+        <v>7.3</v>
+      </c>
+      <c r="D603" t="s">
+        <v>12</v>
+      </c>
+      <c r="E603" s="1">
+        <f>AVERAGE(360,1044)</f>
+        <v>702</v>
+      </c>
+      <c r="F603" s="1">
+        <v>7</v>
+      </c>
+      <c r="G603" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="604" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A604" t="s">
+        <v>7</v>
+      </c>
+      <c r="B604">
+        <v>5</v>
+      </c>
+      <c r="C604">
+        <v>7.3</v>
+      </c>
+      <c r="D604" t="s">
+        <v>18</v>
+      </c>
+      <c r="E604" s="1">
+        <f>AVERAGE(1189,2514)</f>
+        <v>1851.5</v>
+      </c>
+      <c r="F604" s="1">
+        <v>7</v>
+      </c>
+      <c r="G604" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="605" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A605" t="s">
+        <v>7</v>
+      </c>
+      <c r="B605">
+        <v>6.1</v>
+      </c>
+      <c r="C605">
+        <v>7.9</v>
+      </c>
+      <c r="D605" t="s">
+        <v>12</v>
+      </c>
+      <c r="E605" s="1">
+        <f>AVERAGE(396,916)</f>
+        <v>656</v>
+      </c>
+      <c r="F605" s="1">
+        <v>8</v>
+      </c>
+      <c r="G605" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="606" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A606" t="s">
+        <v>7</v>
+      </c>
+      <c r="B606">
+        <v>6.1</v>
+      </c>
+      <c r="C606">
+        <v>7.9</v>
+      </c>
+      <c r="D606" t="s">
+        <v>18</v>
+      </c>
+      <c r="E606" s="1">
+        <f>AVERAGE(1299,2055)</f>
+        <v>1677</v>
+      </c>
+      <c r="F606" s="1">
+        <v>8</v>
+      </c>
+      <c r="G606" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="607" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A607" t="s">
+        <v>7</v>
+      </c>
+      <c r="B607">
+        <v>5</v>
+      </c>
+      <c r="C607">
+        <v>7</v>
+      </c>
+      <c r="D607" t="s">
+        <v>12</v>
+      </c>
+      <c r="E607" s="1">
+        <f>AVERAGE(360,1027)</f>
+        <v>693.5</v>
+      </c>
+      <c r="F607" s="1">
+        <v>90</v>
+      </c>
+      <c r="G607" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="608" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A608" t="s">
+        <v>7</v>
+      </c>
+      <c r="B608">
+        <v>5</v>
+      </c>
+      <c r="C608">
+        <v>7</v>
+      </c>
+      <c r="D608" t="s">
+        <v>18</v>
+      </c>
+      <c r="E608" s="1">
+        <f>AVERAGE(1181,2090)</f>
+        <v>1635.5</v>
+      </c>
+      <c r="F608" s="1">
+        <v>90</v>
+      </c>
+      <c r="G608" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="609" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A609" t="s">
+        <v>1</v>
+      </c>
+      <c r="B609">
+        <v>17</v>
+      </c>
+      <c r="C609">
+        <v>26</v>
+      </c>
+      <c r="D609" t="s">
+        <v>10</v>
+      </c>
+      <c r="E609" s="1">
+        <v>62</v>
+      </c>
+      <c r="F609" s="1">
+        <v>157</v>
+      </c>
+      <c r="G609" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="610" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A610" t="s">
+        <v>1</v>
+      </c>
+      <c r="B610">
+        <v>17</v>
+      </c>
+      <c r="C610">
+        <v>26</v>
+      </c>
+      <c r="D610" t="s">
+        <v>9</v>
+      </c>
+      <c r="E610" s="1">
+        <v>392</v>
+      </c>
+      <c r="F610" s="1">
+        <v>157</v>
+      </c>
+      <c r="G610" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -14830,9 +15167,13 @@
     <hyperlink ref="G23:G24" r:id="rId46" display="https://doi.org/10.1044/2015_AJSLP-15-0020" xr:uid="{B24C93BF-6FB5-8A41-AF83-5523FD1896F5}"/>
     <hyperlink ref="G509" r:id="rId47" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/S0892-1997(99)80011-3" xr:uid="{D7089C36-C646-C24E-8461-A834CF69C5DA}"/>
     <hyperlink ref="G510:G512" r:id="rId48" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/S0892-1997(99)80011-3" xr:uid="{0AE3F141-6ABA-384C-8F34-4564C75A4524}"/>
+    <hyperlink ref="G597" r:id="rId49" display="https://doi.org/10.1121/1.1913429" xr:uid="{80F23F14-09DC-774E-A036-1BA577772636}"/>
+    <hyperlink ref="G598:G602" r:id="rId50" display="https://doi.org/10.1121/1.1913429" xr:uid="{72593115-59D8-D34E-B819-DD67EED70309}"/>
+    <hyperlink ref="G609" xr:uid="{414D9B66-1C24-0E4B-A97A-81B9CFB7A910}"/>
+    <hyperlink ref="G610" xr:uid="{11DCF5ED-A8B8-D14D-B1E1-223066576823}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId49"/>
+  <legacyDrawing r:id="rId51"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
One more (LTAS) formant frequency data set for adults
</commit_message>
<xml_diff>
--- a/inst/default_parameters.xlsx
+++ b/inst/default_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frkkan96/Documents/src/reindeer/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FEC622-9800-5540-B7B1-3420106DE4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1AC63E-4E80-5B4B-80BA-EB2A7114FD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25620" yWindow="500" windowWidth="25580" windowHeight="28300" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1837" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1873" uniqueCount="61">
   <si>
     <t>Gender</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>10.1016/s0095-4470(19)31416-0 </t>
+  </si>
+  <si>
+    <t>10.1044/1092-4388(2003/054)</t>
   </si>
 </sst>
 </file>
@@ -646,10 +649,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3287FC8-0847-0B47-A33C-7A45B3569376}">
-  <dimension ref="A1:G610"/>
+  <dimension ref="A1:G622"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A580" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
-      <selection activeCell="B589" sqref="B589"/>
+    <sheetView tabSelected="1" topLeftCell="A593" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
+      <selection activeCell="G611" sqref="G611:G622"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15115,6 +15118,282 @@
       </c>
       <c r="G610" s="2" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="611" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A611" t="s">
+        <v>1</v>
+      </c>
+      <c r="B611">
+        <v>18</v>
+      </c>
+      <c r="C611">
+        <v>30</v>
+      </c>
+      <c r="D611" t="s">
+        <v>12</v>
+      </c>
+      <c r="E611" s="1">
+        <v>586</v>
+      </c>
+      <c r="F611" s="1">
+        <v>19</v>
+      </c>
+      <c r="G611" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="612" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A612" t="s">
+        <v>1</v>
+      </c>
+      <c r="B612">
+        <v>18</v>
+      </c>
+      <c r="C612">
+        <v>30</v>
+      </c>
+      <c r="D612" t="s">
+        <v>18</v>
+      </c>
+      <c r="E612" s="1">
+        <v>1559</v>
+      </c>
+      <c r="F612" s="1">
+        <v>19</v>
+      </c>
+      <c r="G612" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="613" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A613" t="s">
+        <v>1</v>
+      </c>
+      <c r="B613">
+        <v>18</v>
+      </c>
+      <c r="C613">
+        <v>30</v>
+      </c>
+      <c r="D613" t="s">
+        <v>17</v>
+      </c>
+      <c r="E613" s="1">
+        <v>2384</v>
+      </c>
+      <c r="F613" s="1">
+        <v>19</v>
+      </c>
+      <c r="G613" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="614" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A614" t="s">
+        <v>5</v>
+      </c>
+      <c r="B614">
+        <v>20</v>
+      </c>
+      <c r="C614">
+        <v>30</v>
+      </c>
+      <c r="D614" t="s">
+        <v>12</v>
+      </c>
+      <c r="E614" s="1">
+        <v>580</v>
+      </c>
+      <c r="F614" s="1">
+        <v>19</v>
+      </c>
+      <c r="G614" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="615" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A615" t="s">
+        <v>5</v>
+      </c>
+      <c r="B615">
+        <v>20</v>
+      </c>
+      <c r="C615">
+        <v>30</v>
+      </c>
+      <c r="D615" t="s">
+        <v>18</v>
+      </c>
+      <c r="E615" s="1">
+        <v>1590</v>
+      </c>
+      <c r="F615" s="1">
+        <v>19</v>
+      </c>
+      <c r="G615" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="616" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A616" t="s">
+        <v>5</v>
+      </c>
+      <c r="B616">
+        <v>20</v>
+      </c>
+      <c r="C616">
+        <v>30</v>
+      </c>
+      <c r="D616" t="s">
+        <v>17</v>
+      </c>
+      <c r="E616" s="1">
+        <v>2432</v>
+      </c>
+      <c r="F616" s="1">
+        <v>19</v>
+      </c>
+      <c r="G616" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="617" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A617" t="s">
+        <v>1</v>
+      </c>
+      <c r="B617">
+        <v>62</v>
+      </c>
+      <c r="C617">
+        <v>79</v>
+      </c>
+      <c r="D617" t="s">
+        <v>12</v>
+      </c>
+      <c r="E617" s="1">
+        <v>580</v>
+      </c>
+      <c r="F617" s="1">
+        <v>19</v>
+      </c>
+      <c r="G617" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="618" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A618" t="s">
+        <v>1</v>
+      </c>
+      <c r="B618">
+        <v>62</v>
+      </c>
+      <c r="C618">
+        <v>79</v>
+      </c>
+      <c r="D618" t="s">
+        <v>18</v>
+      </c>
+      <c r="E618" s="1">
+        <v>1551</v>
+      </c>
+      <c r="F618" s="1">
+        <v>19</v>
+      </c>
+      <c r="G618" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="619" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A619" t="s">
+        <v>1</v>
+      </c>
+      <c r="B619">
+        <v>62</v>
+      </c>
+      <c r="C619">
+        <v>79</v>
+      </c>
+      <c r="D619" t="s">
+        <v>17</v>
+      </c>
+      <c r="E619" s="1">
+        <v>2377</v>
+      </c>
+      <c r="F619" s="1">
+        <v>19</v>
+      </c>
+      <c r="G619" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="620" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A620" t="s">
+        <v>5</v>
+      </c>
+      <c r="B620">
+        <v>65</v>
+      </c>
+      <c r="C620">
+        <v>87</v>
+      </c>
+      <c r="D620" t="s">
+        <v>12</v>
+      </c>
+      <c r="E620" s="1">
+        <v>561</v>
+      </c>
+      <c r="F620" s="1">
+        <v>19</v>
+      </c>
+      <c r="G620" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="621" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A621" t="s">
+        <v>5</v>
+      </c>
+      <c r="B621">
+        <v>65</v>
+      </c>
+      <c r="C621">
+        <v>87</v>
+      </c>
+      <c r="D621" t="s">
+        <v>18</v>
+      </c>
+      <c r="E621" s="1">
+        <v>1547</v>
+      </c>
+      <c r="F621" s="1">
+        <v>19</v>
+      </c>
+      <c r="G621" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="622" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A622" t="s">
+        <v>5</v>
+      </c>
+      <c r="B622">
+        <v>65</v>
+      </c>
+      <c r="C622">
+        <v>87</v>
+      </c>
+      <c r="D622" t="s">
+        <v>17</v>
+      </c>
+      <c r="E622" s="1">
+        <v>2393</v>
+      </c>
+      <c r="F622" s="1">
+        <v>19</v>
+      </c>
+      <c r="G622" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -15169,8 +15448,8 @@
     <hyperlink ref="G510:G512" r:id="rId48" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/S0892-1997(99)80011-3" xr:uid="{0AE3F141-6ABA-384C-8F34-4564C75A4524}"/>
     <hyperlink ref="G597" r:id="rId49" display="https://doi.org/10.1121/1.1913429" xr:uid="{80F23F14-09DC-774E-A036-1BA577772636}"/>
     <hyperlink ref="G598:G602" r:id="rId50" display="https://doi.org/10.1121/1.1913429" xr:uid="{72593115-59D8-D34E-B819-DD67EED70309}"/>
-    <hyperlink ref="G609" xr:uid="{414D9B66-1C24-0E4B-A97A-81B9CFB7A910}"/>
-    <hyperlink ref="G610" xr:uid="{11DCF5ED-A8B8-D14D-B1E1-223066576823}"/>
+    <hyperlink ref="G609" display="10.1016/s0095-4470(19)31416-0 " xr:uid="{414D9B66-1C24-0E4B-A97A-81B9CFB7A910}"/>
+    <hyperlink ref="G610" display="10.1016/s0095-4470(19)31416-0 " xr:uid="{11DCF5ED-A8B8-D14D-B1E1-223066576823}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Updated defaults data set.
</commit_message>
<xml_diff>
--- a/inst/default_parameters.xlsx
+++ b/inst/default_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frkkan96/Documents/src/reindeer/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1AC63E-4E80-5B4B-80BA-EB2A7114FD3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18DC021-F831-A149-96F9-2718CB0CA6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25620" yWindow="500" windowWidth="25580" windowHeight="28300" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
+    <workbookView xWindow="38420" yWindow="500" windowWidth="38380" windowHeight="42700" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1873" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="63">
   <si>
     <t>Gender</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>10.1044/1092-4388(2003/054)</t>
+  </si>
+  <si>
+    <t>10.1515/lingvan-2020-0051</t>
+  </si>
+  <si>
+    <t>10.1121/1.411872</t>
   </si>
 </sst>
 </file>
@@ -649,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3287FC8-0847-0B47-A33C-7A45B3569376}">
-  <dimension ref="A1:G622"/>
+  <dimension ref="A1:G638"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A593" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
-      <selection activeCell="G611" sqref="G611:G622"/>
+    <sheetView tabSelected="1" topLeftCell="A608" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
+      <selection activeCell="G630" sqref="G630"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2276,7 +2282,7 @@
         <v>32</v>
       </c>
       <c r="E69" s="1">
-        <v>5200</v>
+        <v>5230</v>
       </c>
       <c r="F69" s="1">
         <v>20</v>
@@ -2299,7 +2305,7 @@
         <v>32</v>
       </c>
       <c r="E70" s="1">
-        <v>6300</v>
+        <v>6000</v>
       </c>
       <c r="F70" s="1">
         <v>20</v>
@@ -15394,6 +15400,386 @@
       </c>
       <c r="G622" s="2" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="623" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A623" t="s">
+        <v>1</v>
+      </c>
+      <c r="B623">
+        <v>20</v>
+      </c>
+      <c r="C623">
+        <v>60</v>
+      </c>
+      <c r="D623" t="s">
+        <v>32</v>
+      </c>
+      <c r="E623" s="1">
+        <v>5230</v>
+      </c>
+      <c r="F623" s="1">
+        <v>45</v>
+      </c>
+      <c r="G623" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="624" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A624" t="s">
+        <v>5</v>
+      </c>
+      <c r="B624">
+        <v>20</v>
+      </c>
+      <c r="C624">
+        <v>60</v>
+      </c>
+      <c r="D624" t="s">
+        <v>32</v>
+      </c>
+      <c r="E624" s="1">
+        <v>6000</v>
+      </c>
+      <c r="F624" s="1">
+        <v>48</v>
+      </c>
+      <c r="G624" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="625" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A625" t="s">
+        <v>1</v>
+      </c>
+      <c r="B625">
+        <v>10</v>
+      </c>
+      <c r="C625">
+        <v>12</v>
+      </c>
+      <c r="D625" t="s">
+        <v>32</v>
+      </c>
+      <c r="E625" s="1">
+        <v>6300</v>
+      </c>
+      <c r="F625" s="1">
+        <v>27</v>
+      </c>
+      <c r="G625" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="626" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A626" t="s">
+        <v>5</v>
+      </c>
+      <c r="B626">
+        <v>10</v>
+      </c>
+      <c r="C626">
+        <v>12</v>
+      </c>
+      <c r="D626" t="s">
+        <v>32</v>
+      </c>
+      <c r="E626" s="1">
+        <v>6500</v>
+      </c>
+      <c r="F626" s="1">
+        <v>19</v>
+      </c>
+      <c r="G626" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="627" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A627" t="s">
+        <v>1</v>
+      </c>
+      <c r="B627">
+        <v>20</v>
+      </c>
+      <c r="C627">
+        <v>60</v>
+      </c>
+      <c r="D627" t="s">
+        <v>12</v>
+      </c>
+      <c r="E627" s="1">
+        <f>AVERAGE(342,768)</f>
+        <v>555</v>
+      </c>
+      <c r="F627" s="1">
+        <v>45</v>
+      </c>
+      <c r="G627" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="628" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A628" t="s">
+        <v>1</v>
+      </c>
+      <c r="B628">
+        <v>20</v>
+      </c>
+      <c r="C628">
+        <v>60</v>
+      </c>
+      <c r="D628" t="s">
+        <v>18</v>
+      </c>
+      <c r="E628" s="1">
+        <f>AVERAGE(2322,910)</f>
+        <v>1616</v>
+      </c>
+      <c r="F628" s="1">
+        <v>45</v>
+      </c>
+      <c r="G628" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="629" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A629" t="s">
+        <v>1</v>
+      </c>
+      <c r="B629">
+        <v>20</v>
+      </c>
+      <c r="C629">
+        <v>60</v>
+      </c>
+      <c r="D629" t="s">
+        <v>17</v>
+      </c>
+      <c r="E629" s="1">
+        <f>AVERAGE(3000,1710)</f>
+        <v>2355</v>
+      </c>
+      <c r="F629" s="1">
+        <v>45</v>
+      </c>
+      <c r="G629" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="630" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A630" t="s">
+        <v>5</v>
+      </c>
+      <c r="B630">
+        <v>20</v>
+      </c>
+      <c r="C630">
+        <v>60</v>
+      </c>
+      <c r="D630" t="s">
+        <v>12</v>
+      </c>
+      <c r="E630" s="1">
+        <f>AVERAGE(936,437)</f>
+        <v>686.5</v>
+      </c>
+      <c r="F630" s="1">
+        <v>48</v>
+      </c>
+      <c r="G630" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="631" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A631" t="s">
+        <v>5</v>
+      </c>
+      <c r="B631">
+        <v>20</v>
+      </c>
+      <c r="C631">
+        <v>60</v>
+      </c>
+      <c r="D631" t="s">
+        <v>18</v>
+      </c>
+      <c r="E631" s="1">
+        <f>AVERAGE(2761,1035)</f>
+        <v>1898</v>
+      </c>
+      <c r="F631" s="1">
+        <v>48</v>
+      </c>
+      <c r="G631" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="632" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A632" t="s">
+        <v>5</v>
+      </c>
+      <c r="B632">
+        <v>20</v>
+      </c>
+      <c r="C632">
+        <v>60</v>
+      </c>
+      <c r="D632" t="s">
+        <v>17</v>
+      </c>
+      <c r="E632" s="1">
+        <f>AVERAGE(3372,1929)</f>
+        <v>2650.5</v>
+      </c>
+      <c r="F632" s="1">
+        <v>48</v>
+      </c>
+      <c r="G632" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="633" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A633" t="s">
+        <v>1</v>
+      </c>
+      <c r="B633">
+        <v>10</v>
+      </c>
+      <c r="C633">
+        <v>12</v>
+      </c>
+      <c r="D633" t="s">
+        <v>12</v>
+      </c>
+      <c r="E633" s="1">
+        <f>AVERAGE(452,1002)</f>
+        <v>727</v>
+      </c>
+      <c r="F633" s="1">
+        <v>27</v>
+      </c>
+      <c r="G633" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="634" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A634" t="s">
+        <v>1</v>
+      </c>
+      <c r="B634">
+        <v>10</v>
+      </c>
+      <c r="C634">
+        <v>12</v>
+      </c>
+      <c r="D634" t="s">
+        <v>18</v>
+      </c>
+      <c r="E634" s="1">
+        <f>AVERAGE(3081,1137)</f>
+        <v>2109</v>
+      </c>
+      <c r="F634" s="1">
+        <v>27</v>
+      </c>
+      <c r="G634" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="635" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A635" t="s">
+        <v>1</v>
+      </c>
+      <c r="B635">
+        <v>10</v>
+      </c>
+      <c r="C635">
+        <v>12</v>
+      </c>
+      <c r="D635" t="s">
+        <v>17</v>
+      </c>
+      <c r="E635" s="1">
+        <f>AVERAGE(3702,2950)</f>
+        <v>3326</v>
+      </c>
+      <c r="F635" s="1">
+        <v>27</v>
+      </c>
+      <c r="G635" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="636" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A636" t="s">
+        <v>5</v>
+      </c>
+      <c r="B636">
+        <v>10</v>
+      </c>
+      <c r="C636">
+        <v>12</v>
+      </c>
+      <c r="D636" t="s">
+        <v>12</v>
+      </c>
+      <c r="E636" s="1">
+        <f>AVERAGE(452,1002)</f>
+        <v>727</v>
+      </c>
+      <c r="F636" s="1">
+        <v>19</v>
+      </c>
+      <c r="G636" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="637" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A637" t="s">
+        <v>5</v>
+      </c>
+      <c r="B637">
+        <v>10</v>
+      </c>
+      <c r="C637">
+        <v>12</v>
+      </c>
+      <c r="D637" t="s">
+        <v>18</v>
+      </c>
+      <c r="E637" s="1">
+        <f>AVERAGE(3081,1137)</f>
+        <v>2109</v>
+      </c>
+      <c r="F637" s="1">
+        <v>19</v>
+      </c>
+      <c r="G637" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="638" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A638" t="s">
+        <v>5</v>
+      </c>
+      <c r="B638">
+        <v>10</v>
+      </c>
+      <c r="C638">
+        <v>12</v>
+      </c>
+      <c r="D638" t="s">
+        <v>17</v>
+      </c>
+      <c r="E638" s="1">
+        <f>AVERAGE(3702,2950)</f>
+        <v>3326</v>
+      </c>
+      <c r="F638" s="1">
+        <v>19</v>
+      </c>
+      <c r="G638" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more data to the collection of settings
</commit_message>
<xml_diff>
--- a/inst/default_parameters.xlsx
+++ b/inst/default_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frkkan96/Documents/src/reindeer/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A18DC021-F831-A149-96F9-2718CB0CA6B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCFF5EB-3DD6-6246-8B19-37F51BD23D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38420" yWindow="500" windowWidth="38380" windowHeight="42700" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="64">
   <si>
     <t>Gender</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t>10.1121/1.411872</t>
+  </si>
+  <si>
+    <t>10.1016/j.neures.2011.01.010</t>
   </si>
 </sst>
 </file>
@@ -655,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3287FC8-0847-0B47-A33C-7A45B3569376}">
-  <dimension ref="A1:G638"/>
+  <dimension ref="A1:G640"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A608" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
-      <selection activeCell="G630" sqref="G630"/>
+    <sheetView tabSelected="1" topLeftCell="A607" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
+      <selection activeCell="D633" sqref="D633"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15780,6 +15783,52 @@
       </c>
       <c r="G638" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="639" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A639" t="s">
+        <v>5</v>
+      </c>
+      <c r="B639">
+        <v>30</v>
+      </c>
+      <c r="C639">
+        <v>40</v>
+      </c>
+      <c r="D639" t="s">
+        <v>10</v>
+      </c>
+      <c r="E639" s="1">
+        <v>100</v>
+      </c>
+      <c r="F639" s="1">
+        <v>24</v>
+      </c>
+      <c r="G639" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="640" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A640" t="s">
+        <v>5</v>
+      </c>
+      <c r="B640">
+        <v>30</v>
+      </c>
+      <c r="C640">
+        <v>40</v>
+      </c>
+      <c r="D640" t="s">
+        <v>9</v>
+      </c>
+      <c r="E640" s="1">
+        <v>420</v>
+      </c>
+      <c r="F640" s="1">
+        <v>24</v>
+      </c>
+      <c r="G640" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the get_parameters function to precompute the DSPP - parameters into a table with Age and Gender defaults in columns
* This change makes metadata_parameters obsolete
</commit_message>
<xml_diff>
--- a/inst/default_parameters.xlsx
+++ b/inst/default_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frkkan96/Documents/src/reindeer/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06005C58-41AC-2943-BEC1-F6DA9B9FED38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B9CAD0A-28DB-6246-82D4-C9BC2838C359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38420" yWindow="500" windowWidth="38380" windowHeight="42700" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{CA423860-348E-DA42-A242-A460E06CAE20}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3287FC8-0847-0B47-A33C-7A45B3569376}">
   <dimension ref="A1:G637"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="210" zoomScaleNormal="207" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -928,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>120</v>
@@ -951,7 +951,7 @@
         <v>3</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>120</v>
@@ -974,7 +974,7 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <v>120</v>
@@ -5618,7 +5618,7 @@
         <v>70</v>
       </c>
       <c r="C207">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D207" t="s">
         <v>8</v>
@@ -5642,7 +5642,7 @@
         <v>70</v>
       </c>
       <c r="C208">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D208" t="s">
         <v>14</v>
@@ -5666,7 +5666,7 @@
         <v>70</v>
       </c>
       <c r="C209">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D209" t="s">
         <v>13</v>
@@ -5834,7 +5834,7 @@
         <v>70</v>
       </c>
       <c r="C216">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D216" t="s">
         <v>8</v>
@@ -5858,7 +5858,7 @@
         <v>70</v>
       </c>
       <c r="C217">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D217" t="s">
         <v>14</v>
@@ -5882,7 +5882,7 @@
         <v>70</v>
       </c>
       <c r="C218">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D218" t="s">
         <v>13</v>
@@ -6122,7 +6122,7 @@
         <v>18</v>
       </c>
       <c r="C228">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D228" t="s">
         <v>8</v>
@@ -6146,7 +6146,7 @@
         <v>18</v>
       </c>
       <c r="C229">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D229" t="s">
         <v>14</v>
@@ -6170,7 +6170,7 @@
         <v>18</v>
       </c>
       <c r="C230">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D230" t="s">
         <v>13</v>
@@ -6194,7 +6194,7 @@
         <v>18</v>
       </c>
       <c r="C231">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D231" t="s">
         <v>8</v>
@@ -6218,7 +6218,7 @@
         <v>18</v>
       </c>
       <c r="C232">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D232" t="s">
         <v>14</v>
@@ -6242,7 +6242,7 @@
         <v>18</v>
       </c>
       <c r="C233">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D233" t="s">
         <v>13</v>

</xml_diff>